<commit_message>
chore: update reports (2025-09-24)
</commit_message>
<xml_diff>
--- a/sol_master_LIVE.xlsx
+++ b/sol_master_LIVE.xlsx
@@ -10256,7 +10256,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
+          <t>2FSn3q2gFFLvmsV4njXRc3z9ig9ypwY6TFVcBLLepump</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -10330,7 +10330,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
+          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -10404,7 +10404,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
+          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -10478,7 +10478,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
+          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -10552,7 +10552,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
+          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -10626,7 +10626,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
+          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -10700,7 +10700,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
+          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
         </is>
       </c>
       <c r="D217" t="n">
@@ -10774,7 +10774,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
+          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -10922,7 +10922,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
+          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -10996,7 +10996,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
+          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -11070,7 +11070,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
+          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
         </is>
       </c>
       <c r="D222" t="n">
@@ -11144,7 +11144,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
+          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
         </is>
       </c>
       <c r="D223" t="n">
@@ -11218,7 +11218,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
+          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -11292,7 +11292,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
+          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
         </is>
       </c>
       <c r="D225" t="n">
@@ -11366,7 +11366,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
+          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -11440,7 +11440,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
+          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -11514,7 +11514,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
+          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -11588,7 +11588,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
+          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -11662,7 +11662,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
+          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -11736,7 +11736,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
+          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -11810,7 +11810,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
+          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -11884,7 +11884,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -11958,7 +11958,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
+          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -12032,7 +12032,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
+          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -12106,7 +12106,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
+          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -12254,7 +12254,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>2ASXv4uqTmJq3nfkmaBCyCiGuytFaki6CJQhJ7MUpump</t>
+          <t>BoPBfkKgWGSDApzBjLi1RPwxvSoiN4ECTSPBH2qFpump</t>
         </is>
       </c>
       <c r="D238" t="n">
@@ -12328,7 +12328,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>2wKTkGQjG9E2wohcYAiJ8EgD3YfpdYaQheJRQ41zpump</t>
+          <t>3SfAaAK5eFx4Q23VySQq35AESmHQoBjVJnG2CrXbpump</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -12402,7 +12402,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>5hLq2RBNaxv5cT9fK4J7oXsKXLkrPXSFzFSwBBjNpump</t>
+          <t>CMHHKQAvfQZWEtxgWqLmhwrCqzzYikZqbTWPkEcCpump</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -12476,7 +12476,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>52na8Ux7ir91V1v3ziNWkPK3Zx16dFpwa8fStfRzpump</t>
+          <t>xmcjcN35cwPheUALX7v3fczpJcCtAtZ2jgPPJkNYUFA</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -12550,7 +12550,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>CFdm8UxTsTs14zEbyHvmLUjnp2LBUnK4AoQqSkCwpump</t>
+          <t>5BuA8VT8rfUM428FWThNNPE9MYYoZvv7ZtL89dB3pump</t>
         </is>
       </c>
       <c r="D242" t="n">
@@ -12624,7 +12624,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>3nCkzXUKY5eqbeJ3RAx3rmqqbnJHqMc2WFhvXqSJjRQi</t>
+          <t>J5FsJhyV5HTneY9PP4J6fkhiNnQaNQ4BzH4hAbDqeRNL</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -12698,7 +12698,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>9FKZKjcBqMDNk7qFLTZJJZcni2j4ttb7CeFXNc6Npump</t>
+          <t>9FWysHuSHNrQnyJoC7qMbm2cLxjT9ttjqBKFp8tzpump</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -12772,7 +12772,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>8wMLunYiViYiPyiLXmL6BRhv1PkbBe9reZ8Q1bVWpump</t>
+          <t>GWJcHRz6EZ2igjXfSWc7cz7PaJHfu8yMu4SL2Jqxpump</t>
         </is>
       </c>
       <c r="D245" t="n">
@@ -12846,7 +12846,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>8vEMeenH81xTMDKJcuAE3Mvk9yKoo5E7YkwhjhN4pump</t>
+          <t>CBhmj8ZUTMwDmWatE5Y3QHVzo3C5UXNpDg8YcGJMpump</t>
         </is>
       </c>
       <c r="D246" t="n">
@@ -12920,7 +12920,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>DBdWfTToJcg7XfKwsNpV1VG8ZN7XpxrPp9rChkHcpump</t>
+          <t>EWdgTzAvBZwchg89f8CaJvtvc1dVish2Fa38jPGgpump</t>
         </is>
       </c>
       <c r="D247" t="n">
@@ -12994,7 +12994,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>EA2eKDU7hpjgRiW6xUtEReoGcD23KmugthyZCTbTpump</t>
+          <t>6ChfYhYQqZ2AfQbf4NMJUqJFGoNa26Y92hS7Ao9mpump</t>
         </is>
       </c>
       <c r="D248" t="n">
@@ -13068,7 +13068,7 @@
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>5kNbJHK3TyUTF4ra8JSfj1NJYt26bjqDoocJCoyks5aN</t>
+          <t>CDzCp6fTS7K9pYZ1JEDb4ZpQ4B85BTqke9Kcmwpp5q3S</t>
         </is>
       </c>
       <c r="D249" t="n">
@@ -13142,7 +13142,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>DS4XQ4KNTLBzZLw7bsEcNJfjhohrmgWaGE8rTtuypump</t>
+          <t>DD8TeSw8y7Q2D8MKSt47cTbAnAcHTFs6viov48PMFQQG</t>
         </is>
       </c>
       <c r="D250" t="n">
@@ -13216,7 +13216,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>8baLMqCkFeSe7FCAfSguQurPjqfbhaU7sa74ShLsP1j7</t>
+          <t>EpWd13A6dwnE8a4KEQx8XPDtaj7qViKZhhDCkmB7pump</t>
         </is>
       </c>
       <c r="D251" t="n">
@@ -13290,7 +13290,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>EY3dLhAt59kgQtjBGxeu9AVWigLawz5KBLXDcynKpump</t>
+          <t>2ps5iWYb4PW353wiGKb36EmieYGQKnBFjxEueenu2bPw</t>
         </is>
       </c>
       <c r="D252" t="n">
@@ -13364,7 +13364,7 @@
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>9AUEQCPHjMg9T9VTR7Yfcon57vkwQfEMnFyHCqCJpump</t>
+          <t>G9c3H8Hed4ZNnXvw2t9P1uJeXcQDmdn57Qi5UtGGpump</t>
         </is>
       </c>
       <c r="D253" t="n">
@@ -13438,7 +13438,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>ELusVXzUPHyAuPB3M7qemr2Y2KshiWnGXauK17XYpump</t>
+          <t>2BLuupGDF6GWVJYZWB6fyJ75dWXjMzKGWVeN2TGppump</t>
         </is>
       </c>
       <c r="D254" t="n">
@@ -13512,7 +13512,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>AHyRdt9xRMKnppx3Hxb1kNYXvfzdmkPQsybcJuU9pump</t>
+          <t>G114LVxZdHtsCfDuYjqP3u3RgmVTjKS6s8qHsHuKpump</t>
         </is>
       </c>
       <c r="D255" t="n">
@@ -13586,7 +13586,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>Geakz9ViTntF8K9X6SjCEH9ZXGTUucideFVvU7Tvpump</t>
+          <t>B9z8cEWFmc7LvQtjKsaLoKqW5MJmGRCWqs1DPKupCfkk</t>
         </is>
       </c>
       <c r="D256" t="n">
@@ -13660,7 +13660,7 @@
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>7crUi3HvVkcB7t8FhHfZH6foyv1Wtozc2hYcmVyJpump</t>
+          <t>AYMwf7uvzTMnnDrw64zcMjLBGaqrVcSGP8eNKXtdpump</t>
         </is>
       </c>
       <c r="D257" t="n">
@@ -13734,7 +13734,7 @@
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>BS3GAr3ww1X8zgASXvx2rxbsrkF895GRdnaYmPtcpump</t>
+          <t>4NWHUsqene63s56idLAchHC85MgvCucBgCsMjkiZpump</t>
         </is>
       </c>
       <c r="D258" t="n">
@@ -13808,7 +13808,7 @@
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>7ziiLugERop4FHLBNS4pmZJ9mKQCSDUuqE7tLq6G4bwB</t>
+          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
         </is>
       </c>
       <c r="D259" t="n">
@@ -13882,7 +13882,7 @@
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
+          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -18491,7 +18491,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
+          <t>2FSn3q2gFFLvmsV4njXRc3z9ig9ypwY6TFVcBLLepump</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -18511,7 +18511,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
+          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -18531,7 +18531,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
+          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -18551,7 +18551,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
+          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -18571,7 +18571,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
+          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -18591,7 +18591,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
+          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -18611,7 +18611,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
+          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -18631,7 +18631,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
+          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -18671,7 +18671,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
+          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -18691,7 +18691,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
+          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -18711,7 +18711,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
+          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -18731,7 +18731,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
+          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -18751,7 +18751,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
+          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -18771,7 +18771,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
+          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -18791,7 +18791,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
+          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -18811,7 +18811,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
+          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -18831,7 +18831,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
+          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -18851,7 +18851,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
+          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -18871,7 +18871,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
+          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -18891,7 +18891,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
+          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -18911,7 +18911,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
+          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -18931,7 +18931,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -18951,7 +18951,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
+          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -18971,7 +18971,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
+          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -18991,7 +18991,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
+          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -19031,7 +19031,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>2ASXv4uqTmJq3nfkmaBCyCiGuytFaki6CJQhJ7MUpump</t>
+          <t>BoPBfkKgWGSDApzBjLi1RPwxvSoiN4ECTSPBH2qFpump</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -19051,7 +19051,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>2wKTkGQjG9E2wohcYAiJ8EgD3YfpdYaQheJRQ41zpump</t>
+          <t>3SfAaAK5eFx4Q23VySQq35AESmHQoBjVJnG2CrXbpump</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -19071,7 +19071,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>5hLq2RBNaxv5cT9fK4J7oXsKXLkrPXSFzFSwBBjNpump</t>
+          <t>CMHHKQAvfQZWEtxgWqLmhwrCqzzYikZqbTWPkEcCpump</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -19091,7 +19091,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>52na8Ux7ir91V1v3ziNWkPK3Zx16dFpwa8fStfRzpump</t>
+          <t>xmcjcN35cwPheUALX7v3fczpJcCtAtZ2jgPPJkNYUFA</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -19111,7 +19111,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>CFdm8UxTsTs14zEbyHvmLUjnp2LBUnK4AoQqSkCwpump</t>
+          <t>5BuA8VT8rfUM428FWThNNPE9MYYoZvv7ZtL89dB3pump</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -19131,7 +19131,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>3nCkzXUKY5eqbeJ3RAx3rmqqbnJHqMc2WFhvXqSJjRQi</t>
+          <t>J5FsJhyV5HTneY9PP4J6fkhiNnQaNQ4BzH4hAbDqeRNL</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -19151,7 +19151,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>9FKZKjcBqMDNk7qFLTZJJZcni2j4ttb7CeFXNc6Npump</t>
+          <t>9FWysHuSHNrQnyJoC7qMbm2cLxjT9ttjqBKFp8tzpump</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -19171,7 +19171,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>8wMLunYiViYiPyiLXmL6BRhv1PkbBe9reZ8Q1bVWpump</t>
+          <t>GWJcHRz6EZ2igjXfSWc7cz7PaJHfu8yMu4SL2Jqxpump</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -19191,7 +19191,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>8vEMeenH81xTMDKJcuAE3Mvk9yKoo5E7YkwhjhN4pump</t>
+          <t>CBhmj8ZUTMwDmWatE5Y3QHVzo3C5UXNpDg8YcGJMpump</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -19211,7 +19211,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>DBdWfTToJcg7XfKwsNpV1VG8ZN7XpxrPp9rChkHcpump</t>
+          <t>EWdgTzAvBZwchg89f8CaJvtvc1dVish2Fa38jPGgpump</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -19231,7 +19231,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>EA2eKDU7hpjgRiW6xUtEReoGcD23KmugthyZCTbTpump</t>
+          <t>6ChfYhYQqZ2AfQbf4NMJUqJFGoNa26Y92hS7Ao9mpump</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -19251,7 +19251,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>5kNbJHK3TyUTF4ra8JSfj1NJYt26bjqDoocJCoyks5aN</t>
+          <t>CDzCp6fTS7K9pYZ1JEDb4ZpQ4B85BTqke9Kcmwpp5q3S</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -19271,7 +19271,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>DS4XQ4KNTLBzZLw7bsEcNJfjhohrmgWaGE8rTtuypump</t>
+          <t>DD8TeSw8y7Q2D8MKSt47cTbAnAcHTFs6viov48PMFQQG</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -19291,7 +19291,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>8baLMqCkFeSe7FCAfSguQurPjqfbhaU7sa74ShLsP1j7</t>
+          <t>EpWd13A6dwnE8a4KEQx8XPDtaj7qViKZhhDCkmB7pump</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -19311,7 +19311,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>EY3dLhAt59kgQtjBGxeu9AVWigLawz5KBLXDcynKpump</t>
+          <t>2ps5iWYb4PW353wiGKb36EmieYGQKnBFjxEueenu2bPw</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -19331,7 +19331,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>9AUEQCPHjMg9T9VTR7Yfcon57vkwQfEMnFyHCqCJpump</t>
+          <t>G9c3H8Hed4ZNnXvw2t9P1uJeXcQDmdn57Qi5UtGGpump</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -19351,7 +19351,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>ELusVXzUPHyAuPB3M7qemr2Y2KshiWnGXauK17XYpump</t>
+          <t>2BLuupGDF6GWVJYZWB6fyJ75dWXjMzKGWVeN2TGppump</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -19371,7 +19371,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>AHyRdt9xRMKnppx3Hxb1kNYXvfzdmkPQsybcJuU9pump</t>
+          <t>G114LVxZdHtsCfDuYjqP3u3RgmVTjKS6s8qHsHuKpump</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -19391,7 +19391,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Geakz9ViTntF8K9X6SjCEH9ZXGTUucideFVvU7Tvpump</t>
+          <t>B9z8cEWFmc7LvQtjKsaLoKqW5MJmGRCWqs1DPKupCfkk</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -19411,7 +19411,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>7crUi3HvVkcB7t8FhHfZH6foyv1Wtozc2hYcmVyJpump</t>
+          <t>AYMwf7uvzTMnnDrw64zcMjLBGaqrVcSGP8eNKXtdpump</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -19431,7 +19431,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>BS3GAr3ww1X8zgASXvx2rxbsrkF895GRdnaYmPtcpump</t>
+          <t>4NWHUsqene63s56idLAchHC85MgvCucBgCsMjkiZpump</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -19451,12 +19451,12 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>7ziiLugERop4FHLBNS4pmZJ9mKQCSDUuqE7tLq6G4bwB</t>
+          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>DexProfilesLatest</t>
+          <t>Fallback:Master</t>
         </is>
       </c>
     </row>
@@ -19471,7 +19471,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
+          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -19554,7 +19554,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
+          <t>2FSn3q2gFFLvmsV4njXRc3z9ig9ypwY6TFVcBLLepump</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -19572,7 +19572,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
+          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -19590,7 +19590,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
+          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -19608,7 +19608,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
+          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -19626,7 +19626,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
+          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -19644,7 +19644,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
+          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -19662,7 +19662,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
+          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -19680,7 +19680,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
+          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -19716,7 +19716,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
+          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -19734,7 +19734,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
+          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -19752,7 +19752,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
+          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -19770,7 +19770,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
+          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -19788,7 +19788,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
+          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -19806,12 +19806,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
+          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-09-24</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -19824,12 +19824,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
+          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -19842,7 +19842,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
+          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -19860,7 +19860,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
+          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -19878,7 +19878,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
+          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -19896,7 +19896,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
+          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -19914,7 +19914,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
+          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -19932,7 +19932,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
+          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -19950,7 +19950,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -19968,7 +19968,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
+          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -19986,7 +19986,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
+          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -20004,7 +20004,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
+          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -20040,7 +20040,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2ASXv4uqTmJq3nfkmaBCyCiGuytFaki6CJQhJ7MUpump</t>
+          <t>BoPBfkKgWGSDApzBjLi1RPwxvSoiN4ECTSPBH2qFpump</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -20058,7 +20058,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2wKTkGQjG9E2wohcYAiJ8EgD3YfpdYaQheJRQ41zpump</t>
+          <t>3SfAaAK5eFx4Q23VySQq35AESmHQoBjVJnG2CrXbpump</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -20076,7 +20076,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5hLq2RBNaxv5cT9fK4J7oXsKXLkrPXSFzFSwBBjNpump</t>
+          <t>CMHHKQAvfQZWEtxgWqLmhwrCqzzYikZqbTWPkEcCpump</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -20094,7 +20094,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>52na8Ux7ir91V1v3ziNWkPK3Zx16dFpwa8fStfRzpump</t>
+          <t>xmcjcN35cwPheUALX7v3fczpJcCtAtZ2jgPPJkNYUFA</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -20112,7 +20112,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CFdm8UxTsTs14zEbyHvmLUjnp2LBUnK4AoQqSkCwpump</t>
+          <t>5BuA8VT8rfUM428FWThNNPE9MYYoZvv7ZtL89dB3pump</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -20130,7 +20130,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3nCkzXUKY5eqbeJ3RAx3rmqqbnJHqMc2WFhvXqSJjRQi</t>
+          <t>J5FsJhyV5HTneY9PP4J6fkhiNnQaNQ4BzH4hAbDqeRNL</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -20148,7 +20148,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>9FKZKjcBqMDNk7qFLTZJJZcni2j4ttb7CeFXNc6Npump</t>
+          <t>9FWysHuSHNrQnyJoC7qMbm2cLxjT9ttjqBKFp8tzpump</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -20166,7 +20166,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>8wMLunYiViYiPyiLXmL6BRhv1PkbBe9reZ8Q1bVWpump</t>
+          <t>GWJcHRz6EZ2igjXfSWc7cz7PaJHfu8yMu4SL2Jqxpump</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -20184,7 +20184,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>8vEMeenH81xTMDKJcuAE3Mvk9yKoo5E7YkwhjhN4pump</t>
+          <t>CBhmj8ZUTMwDmWatE5Y3QHVzo3C5UXNpDg8YcGJMpump</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -20202,7 +20202,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>DBdWfTToJcg7XfKwsNpV1VG8ZN7XpxrPp9rChkHcpump</t>
+          <t>EWdgTzAvBZwchg89f8CaJvtvc1dVish2Fa38jPGgpump</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -20220,7 +20220,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>EA2eKDU7hpjgRiW6xUtEReoGcD23KmugthyZCTbTpump</t>
+          <t>6ChfYhYQqZ2AfQbf4NMJUqJFGoNa26Y92hS7Ao9mpump</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -20238,7 +20238,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5kNbJHK3TyUTF4ra8JSfj1NJYt26bjqDoocJCoyks5aN</t>
+          <t>CDzCp6fTS7K9pYZ1JEDb4ZpQ4B85BTqke9Kcmwpp5q3S</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -20256,7 +20256,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>DS4XQ4KNTLBzZLw7bsEcNJfjhohrmgWaGE8rTtuypump</t>
+          <t>DD8TeSw8y7Q2D8MKSt47cTbAnAcHTFs6viov48PMFQQG</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -20274,7 +20274,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>8baLMqCkFeSe7FCAfSguQurPjqfbhaU7sa74ShLsP1j7</t>
+          <t>EpWd13A6dwnE8a4KEQx8XPDtaj7qViKZhhDCkmB7pump</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -20292,7 +20292,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>EY3dLhAt59kgQtjBGxeu9AVWigLawz5KBLXDcynKpump</t>
+          <t>2ps5iWYb4PW353wiGKb36EmieYGQKnBFjxEueenu2bPw</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -20310,7 +20310,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>9AUEQCPHjMg9T9VTR7Yfcon57vkwQfEMnFyHCqCJpump</t>
+          <t>G9c3H8Hed4ZNnXvw2t9P1uJeXcQDmdn57Qi5UtGGpump</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -20328,7 +20328,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>ELusVXzUPHyAuPB3M7qemr2Y2KshiWnGXauK17XYpump</t>
+          <t>2BLuupGDF6GWVJYZWB6fyJ75dWXjMzKGWVeN2TGppump</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -20346,7 +20346,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>AHyRdt9xRMKnppx3Hxb1kNYXvfzdmkPQsybcJuU9pump</t>
+          <t>G114LVxZdHtsCfDuYjqP3u3RgmVTjKS6s8qHsHuKpump</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -20364,7 +20364,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Geakz9ViTntF8K9X6SjCEH9ZXGTUucideFVvU7Tvpump</t>
+          <t>B9z8cEWFmc7LvQtjKsaLoKqW5MJmGRCWqs1DPKupCfkk</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -20382,7 +20382,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>7crUi3HvVkcB7t8FhHfZH6foyv1Wtozc2hYcmVyJpump</t>
+          <t>AYMwf7uvzTMnnDrw64zcMjLBGaqrVcSGP8eNKXtdpump</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -20400,7 +20400,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>BS3GAr3ww1X8zgASXvx2rxbsrkF895GRdnaYmPtcpump</t>
+          <t>4NWHUsqene63s56idLAchHC85MgvCucBgCsMjkiZpump</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -20418,7 +20418,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>7ziiLugERop4FHLBNS4pmZJ9mKQCSDUuqE7tLq6G4bwB</t>
+          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -20436,7 +20436,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
+          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -20569,7 +20569,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-09-24T09:03:46.590625</t>
+          <t>2025-09-24T12:29:00.461557</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">

</xml_diff>

<commit_message>
chore: update reports (2025-09-26)
</commit_message>
<xml_diff>
--- a/sol_master_LIVE.xlsx
+++ b/sol_master_LIVE.xlsx
@@ -10251,12 +10251,12 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>2FSn3q2gFFLvmsV4njXRc3z9ig9ypwY6TFVcBLLepump</t>
+          <t>2Mk8vAfersJgfeT5Pwpfe7y4sQ769GZPhRrnwSdhpump</t>
         </is>
       </c>
       <c r="D211" t="n">
@@ -10325,12 +10325,12 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
+          <t>BuTM2tXzmuM6TcS9cTQhL1VaxjDfYtSHgKHkYQsFpRsX</t>
         </is>
       </c>
       <c r="D212" t="n">
@@ -10399,12 +10399,12 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
+          <t>BqndqeBCNSEftBKmbTbLVx1RX5zd5J3AGL9sG55Jpump</t>
         </is>
       </c>
       <c r="D213" t="n">
@@ -10473,12 +10473,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
+          <t>6NdUMfsuyGENe98VPVMRxNZnbQgTUaKxLuiLszS5pump</t>
         </is>
       </c>
       <c r="D214" t="n">
@@ -10547,12 +10547,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
+          <t>oxynABVJXUEc9PLNx4m1XVdiFtRhStzRXG1G6qosni1</t>
         </is>
       </c>
       <c r="D215" t="n">
@@ -10621,12 +10621,12 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
+          <t>EMg2QkFZ6pLvgckVGj8X6nmyrkiuoamYnTdoxXN8pump</t>
         </is>
       </c>
       <c r="D216" t="n">
@@ -10695,12 +10695,12 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
+          <t>AufjSxXopMZn7EeX21ifncGPKQ2BH6FaiRpFu6gDpump</t>
         </is>
       </c>
       <c r="D217" t="n">
@@ -10769,12 +10769,12 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
+          <t>HBukB9DLbdTM6nNHQQ6JvVmjx7UmuMpDJAU9oX8tpump</t>
         </is>
       </c>
       <c r="D218" t="n">
@@ -10843,12 +10843,12 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>34AeqX5MQGyrey2VnZdkeZCfM4qinp4F3X7pGxtipump</t>
+          <t>xxxgjrRmEtAeik3fpkftHA6ncHjfDWWN4T1zUYQPm3z</t>
         </is>
       </c>
       <c r="D219" t="n">
@@ -10917,12 +10917,12 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
+          <t>2t2sKsaGpRG3jWV22y9eAVp7qfRRaytDiS1kkMpCqREV</t>
         </is>
       </c>
       <c r="D220" t="n">
@@ -10991,12 +10991,12 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
+          <t>DiiTPZdpd9t3XorHiuZUu4E1FoSaQ7uGN4q9YkQupump</t>
         </is>
       </c>
       <c r="D221" t="n">
@@ -11065,12 +11065,12 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
+          <t>CKVZPWFPaJArEaPnk16CXpFtFXjuCxCh95vBcS3Ppump</t>
         </is>
       </c>
       <c r="D222" t="n">
@@ -11139,12 +11139,12 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
+          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
         </is>
       </c>
       <c r="D223" t="n">
@@ -11213,12 +11213,12 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
+          <t>6NqgJiWQLVznisyn1ytHEtQkC52sQf4t1b732Qvvpump</t>
         </is>
       </c>
       <c r="D224" t="n">
@@ -11287,12 +11287,12 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
+          <t>EfFvS8CXAJ89Y3hP8cMpmtW1kDWTg4PnhLMkrW29pump</t>
         </is>
       </c>
       <c r="D225" t="n">
@@ -11361,12 +11361,12 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
+          <t>3d3suDtLDqnXyA454EYCkAnhz33P55FAMCEk37Gppump</t>
         </is>
       </c>
       <c r="D226" t="n">
@@ -11435,12 +11435,12 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
+          <t>FjXD9UWJaG6iVhExBR9SC6HjPmFA3czPGLeSbxurpump</t>
         </is>
       </c>
       <c r="D227" t="n">
@@ -11509,12 +11509,12 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
+          <t>irSdJ3vRioPxMmN3ZFrG6Y7ECJtyyJBnUcLKMauA6tR</t>
         </is>
       </c>
       <c r="D228" t="n">
@@ -11583,12 +11583,12 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
+          <t>919MM61rJb1KairDkbNoH8iCVkX1fGFn7w4Dj6Mapump</t>
         </is>
       </c>
       <c r="D229" t="n">
@@ -11657,12 +11657,12 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
+          <t>GEHJx1yb83BDdjWp6UJWWann9aAkVKwvzU49Qp7jpump</t>
         </is>
       </c>
       <c r="D230" t="n">
@@ -11731,12 +11731,12 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
+          <t>4Ds7cxJ82gm34gV22zo2LjPdX3nFbQk9PXK7mjX4pump</t>
         </is>
       </c>
       <c r="D231" t="n">
@@ -11805,12 +11805,12 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
+          <t>3d1qHSAkQhoN7kN1C6tvpAArCkXWxwYdBng6taXCDM6u</t>
         </is>
       </c>
       <c r="D232" t="n">
@@ -11879,12 +11879,12 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
+          <t>CWVuqZzGfrXD5i1dJYyvpLaQW6yzPqaPC7UemZFUpump</t>
         </is>
       </c>
       <c r="D233" t="n">
@@ -11953,12 +11953,12 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
+          <t>8MWLo9PmNiunLFhCZsXBsHqmvKrxTjt3qffFJF81pump</t>
         </is>
       </c>
       <c r="D234" t="n">
@@ -12027,12 +12027,12 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
+          <t>GaPbGp23pPuY9QBLPUjUEBn2MKEroTe9Q3M3f2Xpump</t>
         </is>
       </c>
       <c r="D235" t="n">
@@ -12101,12 +12101,12 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
+          <t>7UgmCpkZMMQBUajCfhrtiJXZ1wPuMidEB4DnA6aUpump</t>
         </is>
       </c>
       <c r="D236" t="n">
@@ -12175,12 +12175,12 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>5t3TrtpDm1P8pRVYXcJ6MmngNsv2Ty3H5cimDve2pump</t>
+          <t>5YesRCpnjAR396xDy1xenHahfogjevCH4c46TH6wPray</t>
         </is>
       </c>
       <c r="D237" t="n">
@@ -12249,12 +12249,12 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>BoPBfkKgWGSDApzBjLi1RPwxvSoiN4ECTSPBH2qFpump</t>
+          <t>A6ec7AMvx7oH96sNYELiF5i3vw3YxCuN6Qb8fDMMpump</t>
         </is>
       </c>
       <c r="D238" t="n">
@@ -12323,12 +12323,12 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>3SfAaAK5eFx4Q23VySQq35AESmHQoBjVJnG2CrXbpump</t>
+          <t>34wfgAa6JzKxN1TGCneRk3LY1xetvnF8q5n6H7fzf2TY</t>
         </is>
       </c>
       <c r="D239" t="n">
@@ -12397,12 +12397,12 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>CMHHKQAvfQZWEtxgWqLmhwrCqzzYikZqbTWPkEcCpump</t>
+          <t>ByC7sCHFL4s96JnwhbnC27dyY9iTzsjYDvx3XGgopump</t>
         </is>
       </c>
       <c r="D240" t="n">
@@ -12471,12 +12471,12 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>xmcjcN35cwPheUALX7v3fczpJcCtAtZ2jgPPJkNYUFA</t>
+          <t>CWdRtpnFWVgTASioj6ZWPwca3j7i3Ya1hPF4QVL6bonk</t>
         </is>
       </c>
       <c r="D241" t="n">
@@ -12545,12 +12545,12 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>5BuA8VT8rfUM428FWThNNPE9MYYoZvv7ZtL89dB3pump</t>
+          <t>AS5DW5dHY9V46Mrz3VJAA2MsewkahDnHvv9tzNcnpump</t>
         </is>
       </c>
       <c r="D242" t="n">
@@ -12619,12 +12619,12 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>J5FsJhyV5HTneY9PP4J6fkhiNnQaNQ4BzH4hAbDqeRNL</t>
+          <t>G9mRRd16qLYzbp7trdj7DFSZyLePM9DepaWnJJLwCUDF</t>
         </is>
       </c>
       <c r="D243" t="n">
@@ -12693,12 +12693,12 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>9FWysHuSHNrQnyJoC7qMbm2cLxjT9ttjqBKFp8tzpump</t>
+          <t>879iULwrP3VoPF7Ce2yxkMagpwecQLKkNtsY7DJrpump</t>
         </is>
       </c>
       <c r="D244" t="n">
@@ -12767,12 +12767,12 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>GWJcHRz6EZ2igjXfSWc7cz7PaJHfu8yMu4SL2Jqxpump</t>
+          <t>62GnkrYtLJBXoQWsCBHZVugkCDZzpBonAWX6CHmSpump</t>
         </is>
       </c>
       <c r="D245" t="n">
@@ -12841,12 +12841,12 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>CBhmj8ZUTMwDmWatE5Y3QHVzo3C5UXNpDg8YcGJMpump</t>
+          <t>3H9TNBGGh3jdBC76VdTJCB5QSSsKBKFnhM7164VnjpkM</t>
         </is>
       </c>
       <c r="D246" t="n">
@@ -12915,12 +12915,12 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>EWdgTzAvBZwchg89f8CaJvtvc1dVish2Fa38jPGgpump</t>
+          <t>BSmKbyHpyWVamsGv6Ja7xEqAyMwNn4TRsyX4hFxEpump</t>
         </is>
       </c>
       <c r="D247" t="n">
@@ -12989,12 +12989,12 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>6ChfYhYQqZ2AfQbf4NMJUqJFGoNa26Y92hS7Ao9mpump</t>
+          <t>C8aogMqASuurkwKDzd6VZPNRqUTbVoDJH7GMiRYUpump</t>
         </is>
       </c>
       <c r="D248" t="n">
@@ -13063,12 +13063,12 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>CDzCp6fTS7K9pYZ1JEDb4ZpQ4B85BTqke9Kcmwpp5q3S</t>
+          <t>DrJnnTuBDLRZTQmtKgcBkFH3taLbGCNh9DBhWMkhpump</t>
         </is>
       </c>
       <c r="D249" t="n">
@@ -13137,12 +13137,12 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>DD8TeSw8y7Q2D8MKSt47cTbAnAcHTFs6viov48PMFQQG</t>
+          <t>4uVEktQLeYdZHKVJP5FXzZLnzetwhfeyP8vyKXurpump</t>
         </is>
       </c>
       <c r="D250" t="n">
@@ -13211,12 +13211,12 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>EpWd13A6dwnE8a4KEQx8XPDtaj7qViKZhhDCkmB7pump</t>
+          <t>8oCqyRtFXjYbeC7fhxQMAqu6eAMEoibjyJCQcLnopump</t>
         </is>
       </c>
       <c r="D251" t="n">
@@ -13285,12 +13285,12 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>2ps5iWYb4PW353wiGKb36EmieYGQKnBFjxEueenu2bPw</t>
+          <t>APbFhZNhR4goT1JbCFiTrw2N5rPckj5kWZLVzRtnBWLc</t>
         </is>
       </c>
       <c r="D252" t="n">
@@ -13359,12 +13359,12 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>G9c3H8Hed4ZNnXvw2t9P1uJeXcQDmdn57Qi5UtGGpump</t>
+          <t>6hKgCdFex2tTevTNokEmwovtGqtSYK2ps4AigmFwbonk</t>
         </is>
       </c>
       <c r="D253" t="n">
@@ -13433,12 +13433,12 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>2BLuupGDF6GWVJYZWB6fyJ75dWXjMzKGWVeN2TGppump</t>
+          <t>gkz69isayhx176GYZDE333gPyKoiAtMF2TGTNZwpump</t>
         </is>
       </c>
       <c r="D254" t="n">
@@ -13507,12 +13507,12 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>G114LVxZdHtsCfDuYjqP3u3RgmVTjKS6s8qHsHuKpump</t>
+          <t>8GRd7Eg6kFJZTvDdRQpRBX7w71s8R1wkQvMV3HWDT9PT</t>
         </is>
       </c>
       <c r="D255" t="n">
@@ -13581,12 +13581,12 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>B9z8cEWFmc7LvQtjKsaLoKqW5MJmGRCWqs1DPKupCfkk</t>
+          <t>FSyuCSheYUgtaSDa9iJVdVjgVf24XwipMLgWmjEbpump</t>
         </is>
       </c>
       <c r="D256" t="n">
@@ -13655,12 +13655,12 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
         <is>
-          <t>AYMwf7uvzTMnnDrw64zcMjLBGaqrVcSGP8eNKXtdpump</t>
+          <t>Dde3kgfE97FSCuYLpQHpJNLRcaFWXt6rnPcTc165pump</t>
         </is>
       </c>
       <c r="D257" t="n">
@@ -13729,12 +13729,12 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
         <is>
-          <t>4NWHUsqene63s56idLAchHC85MgvCucBgCsMjkiZpump</t>
+          <t>8PMg4GeyHCY1AWctg4ByowPSq35Pu9ZJHfNR4nAcbonk</t>
         </is>
       </c>
       <c r="D258" t="n">
@@ -13803,12 +13803,12 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
         <is>
-          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
+          <t>3KuSj5VbdUCaSRXCXiUThNaJYjx4NPBbNNo4zmKzpump</t>
         </is>
       </c>
       <c r="D259" t="n">
@@ -13877,12 +13877,12 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
         <is>
-          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
+          <t>8RwSa8i6sVhdU4KmXatE6syDgSDUEmKiZC6C4KCTpump</t>
         </is>
       </c>
       <c r="D260" t="n">
@@ -18483,7 +18483,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B202" t="n">
@@ -18491,7 +18491,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>2FSn3q2gFFLvmsV4njXRc3z9ig9ypwY6TFVcBLLepump</t>
+          <t>2Mk8vAfersJgfeT5Pwpfe7y4sQ769GZPhRrnwSdhpump</t>
         </is>
       </c>
       <c r="F202" t="inlineStr">
@@ -18503,7 +18503,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B203" t="n">
@@ -18511,7 +18511,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
+          <t>BuTM2tXzmuM6TcS9cTQhL1VaxjDfYtSHgKHkYQsFpRsX</t>
         </is>
       </c>
       <c r="F203" t="inlineStr">
@@ -18523,7 +18523,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B204" t="n">
@@ -18531,7 +18531,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
+          <t>BqndqeBCNSEftBKmbTbLVx1RX5zd5J3AGL9sG55Jpump</t>
         </is>
       </c>
       <c r="F204" t="inlineStr">
@@ -18543,7 +18543,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B205" t="n">
@@ -18551,7 +18551,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
+          <t>6NdUMfsuyGENe98VPVMRxNZnbQgTUaKxLuiLszS5pump</t>
         </is>
       </c>
       <c r="F205" t="inlineStr">
@@ -18563,7 +18563,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B206" t="n">
@@ -18571,7 +18571,7 @@
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
+          <t>oxynABVJXUEc9PLNx4m1XVdiFtRhStzRXG1G6qosni1</t>
         </is>
       </c>
       <c r="F206" t="inlineStr">
@@ -18583,7 +18583,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B207" t="n">
@@ -18591,7 +18591,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
+          <t>EMg2QkFZ6pLvgckVGj8X6nmyrkiuoamYnTdoxXN8pump</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
@@ -18603,7 +18603,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B208" t="n">
@@ -18611,7 +18611,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
+          <t>AufjSxXopMZn7EeX21ifncGPKQ2BH6FaiRpFu6gDpump</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -18623,7 +18623,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B209" t="n">
@@ -18631,7 +18631,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
+          <t>HBukB9DLbdTM6nNHQQ6JvVmjx7UmuMpDJAU9oX8tpump</t>
         </is>
       </c>
       <c r="F209" t="inlineStr">
@@ -18643,7 +18643,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B210" t="n">
@@ -18651,7 +18651,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>34AeqX5MQGyrey2VnZdkeZCfM4qinp4F3X7pGxtipump</t>
+          <t>xxxgjrRmEtAeik3fpkftHA6ncHjfDWWN4T1zUYQPm3z</t>
         </is>
       </c>
       <c r="F210" t="inlineStr">
@@ -18663,7 +18663,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B211" t="n">
@@ -18671,7 +18671,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
+          <t>2t2sKsaGpRG3jWV22y9eAVp7qfRRaytDiS1kkMpCqREV</t>
         </is>
       </c>
       <c r="F211" t="inlineStr">
@@ -18683,7 +18683,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B212" t="n">
@@ -18691,7 +18691,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
+          <t>DiiTPZdpd9t3XorHiuZUu4E1FoSaQ7uGN4q9YkQupump</t>
         </is>
       </c>
       <c r="F212" t="inlineStr">
@@ -18703,7 +18703,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B213" t="n">
@@ -18711,7 +18711,7 @@
       </c>
       <c r="C213" t="inlineStr">
         <is>
-          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
+          <t>CKVZPWFPaJArEaPnk16CXpFtFXjuCxCh95vBcS3Ppump</t>
         </is>
       </c>
       <c r="F213" t="inlineStr">
@@ -18723,7 +18723,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B214" t="n">
@@ -18731,7 +18731,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
+          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
         </is>
       </c>
       <c r="F214" t="inlineStr">
@@ -18743,7 +18743,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B215" t="n">
@@ -18751,7 +18751,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
+          <t>6NqgJiWQLVznisyn1ytHEtQkC52sQf4t1b732Qvvpump</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -18763,7 +18763,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B216" t="n">
@@ -18771,7 +18771,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
+          <t>EfFvS8CXAJ89Y3hP8cMpmtW1kDWTg4PnhLMkrW29pump</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -18783,7 +18783,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B217" t="n">
@@ -18791,7 +18791,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
+          <t>3d3suDtLDqnXyA454EYCkAnhz33P55FAMCEk37Gppump</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -18803,7 +18803,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B218" t="n">
@@ -18811,7 +18811,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
+          <t>FjXD9UWJaG6iVhExBR9SC6HjPmFA3czPGLeSbxurpump</t>
         </is>
       </c>
       <c r="F218" t="inlineStr">
@@ -18823,7 +18823,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B219" t="n">
@@ -18831,7 +18831,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
+          <t>irSdJ3vRioPxMmN3ZFrG6Y7ECJtyyJBnUcLKMauA6tR</t>
         </is>
       </c>
       <c r="F219" t="inlineStr">
@@ -18843,7 +18843,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B220" t="n">
@@ -18851,7 +18851,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
+          <t>919MM61rJb1KairDkbNoH8iCVkX1fGFn7w4Dj6Mapump</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
@@ -18863,7 +18863,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B221" t="n">
@@ -18871,7 +18871,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
+          <t>GEHJx1yb83BDdjWp6UJWWann9aAkVKwvzU49Qp7jpump</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
@@ -18883,7 +18883,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B222" t="n">
@@ -18891,7 +18891,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
+          <t>4Ds7cxJ82gm34gV22zo2LjPdX3nFbQk9PXK7mjX4pump</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
@@ -18903,7 +18903,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B223" t="n">
@@ -18911,7 +18911,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
+          <t>3d1qHSAkQhoN7kN1C6tvpAArCkXWxwYdBng6taXCDM6u</t>
         </is>
       </c>
       <c r="F223" t="inlineStr">
@@ -18923,7 +18923,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B224" t="n">
@@ -18931,7 +18931,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
+          <t>CWVuqZzGfrXD5i1dJYyvpLaQW6yzPqaPC7UemZFUpump</t>
         </is>
       </c>
       <c r="F224" t="inlineStr">
@@ -18943,7 +18943,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B225" t="n">
@@ -18951,7 +18951,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
+          <t>8MWLo9PmNiunLFhCZsXBsHqmvKrxTjt3qffFJF81pump</t>
         </is>
       </c>
       <c r="F225" t="inlineStr">
@@ -18963,7 +18963,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B226" t="n">
@@ -18971,7 +18971,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
+          <t>GaPbGp23pPuY9QBLPUjUEBn2MKEroTe9Q3M3f2Xpump</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -18983,7 +18983,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B227" t="n">
@@ -18991,7 +18991,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
+          <t>7UgmCpkZMMQBUajCfhrtiJXZ1wPuMidEB4DnA6aUpump</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
@@ -19003,7 +19003,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B228" t="n">
@@ -19011,7 +19011,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>5t3TrtpDm1P8pRVYXcJ6MmngNsv2Ty3H5cimDve2pump</t>
+          <t>5YesRCpnjAR396xDy1xenHahfogjevCH4c46TH6wPray</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
@@ -19023,7 +19023,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B229" t="n">
@@ -19031,7 +19031,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>BoPBfkKgWGSDApzBjLi1RPwxvSoiN4ECTSPBH2qFpump</t>
+          <t>A6ec7AMvx7oH96sNYELiF5i3vw3YxCuN6Qb8fDMMpump</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
@@ -19043,7 +19043,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B230" t="n">
@@ -19051,7 +19051,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>3SfAaAK5eFx4Q23VySQq35AESmHQoBjVJnG2CrXbpump</t>
+          <t>34wfgAa6JzKxN1TGCneRk3LY1xetvnF8q5n6H7fzf2TY</t>
         </is>
       </c>
       <c r="F230" t="inlineStr">
@@ -19063,7 +19063,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B231" t="n">
@@ -19071,7 +19071,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>CMHHKQAvfQZWEtxgWqLmhwrCqzzYikZqbTWPkEcCpump</t>
+          <t>ByC7sCHFL4s96JnwhbnC27dyY9iTzsjYDvx3XGgopump</t>
         </is>
       </c>
       <c r="F231" t="inlineStr">
@@ -19083,7 +19083,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B232" t="n">
@@ -19091,7 +19091,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>xmcjcN35cwPheUALX7v3fczpJcCtAtZ2jgPPJkNYUFA</t>
+          <t>CWdRtpnFWVgTASioj6ZWPwca3j7i3Ya1hPF4QVL6bonk</t>
         </is>
       </c>
       <c r="F232" t="inlineStr">
@@ -19103,7 +19103,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B233" t="n">
@@ -19111,7 +19111,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>5BuA8VT8rfUM428FWThNNPE9MYYoZvv7ZtL89dB3pump</t>
+          <t>AS5DW5dHY9V46Mrz3VJAA2MsewkahDnHvv9tzNcnpump</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -19123,7 +19123,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B234" t="n">
@@ -19131,7 +19131,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>J5FsJhyV5HTneY9PP4J6fkhiNnQaNQ4BzH4hAbDqeRNL</t>
+          <t>G9mRRd16qLYzbp7trdj7DFSZyLePM9DepaWnJJLwCUDF</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -19143,7 +19143,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B235" t="n">
@@ -19151,7 +19151,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>9FWysHuSHNrQnyJoC7qMbm2cLxjT9ttjqBKFp8tzpump</t>
+          <t>879iULwrP3VoPF7Ce2yxkMagpwecQLKkNtsY7DJrpump</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -19163,7 +19163,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B236" t="n">
@@ -19171,7 +19171,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>GWJcHRz6EZ2igjXfSWc7cz7PaJHfu8yMu4SL2Jqxpump</t>
+          <t>62GnkrYtLJBXoQWsCBHZVugkCDZzpBonAWX6CHmSpump</t>
         </is>
       </c>
       <c r="F236" t="inlineStr">
@@ -19183,7 +19183,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B237" t="n">
@@ -19191,7 +19191,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>CBhmj8ZUTMwDmWatE5Y3QHVzo3C5UXNpDg8YcGJMpump</t>
+          <t>3H9TNBGGh3jdBC76VdTJCB5QSSsKBKFnhM7164VnjpkM</t>
         </is>
       </c>
       <c r="F237" t="inlineStr">
@@ -19203,7 +19203,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B238" t="n">
@@ -19211,7 +19211,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>EWdgTzAvBZwchg89f8CaJvtvc1dVish2Fa38jPGgpump</t>
+          <t>BSmKbyHpyWVamsGv6Ja7xEqAyMwNn4TRsyX4hFxEpump</t>
         </is>
       </c>
       <c r="F238" t="inlineStr">
@@ -19223,7 +19223,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B239" t="n">
@@ -19231,7 +19231,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>6ChfYhYQqZ2AfQbf4NMJUqJFGoNa26Y92hS7Ao9mpump</t>
+          <t>C8aogMqASuurkwKDzd6VZPNRqUTbVoDJH7GMiRYUpump</t>
         </is>
       </c>
       <c r="F239" t="inlineStr">
@@ -19243,7 +19243,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B240" t="n">
@@ -19251,7 +19251,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>CDzCp6fTS7K9pYZ1JEDb4ZpQ4B85BTqke9Kcmwpp5q3S</t>
+          <t>DrJnnTuBDLRZTQmtKgcBkFH3taLbGCNh9DBhWMkhpump</t>
         </is>
       </c>
       <c r="F240" t="inlineStr">
@@ -19263,7 +19263,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B241" t="n">
@@ -19271,7 +19271,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>DD8TeSw8y7Q2D8MKSt47cTbAnAcHTFs6viov48PMFQQG</t>
+          <t>4uVEktQLeYdZHKVJP5FXzZLnzetwhfeyP8vyKXurpump</t>
         </is>
       </c>
       <c r="F241" t="inlineStr">
@@ -19283,7 +19283,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B242" t="n">
@@ -19291,7 +19291,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>EpWd13A6dwnE8a4KEQx8XPDtaj7qViKZhhDCkmB7pump</t>
+          <t>8oCqyRtFXjYbeC7fhxQMAqu6eAMEoibjyJCQcLnopump</t>
         </is>
       </c>
       <c r="F242" t="inlineStr">
@@ -19303,7 +19303,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B243" t="n">
@@ -19311,7 +19311,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>2ps5iWYb4PW353wiGKb36EmieYGQKnBFjxEueenu2bPw</t>
+          <t>APbFhZNhR4goT1JbCFiTrw2N5rPckj5kWZLVzRtnBWLc</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -19323,7 +19323,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B244" t="n">
@@ -19331,7 +19331,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>G9c3H8Hed4ZNnXvw2t9P1uJeXcQDmdn57Qi5UtGGpump</t>
+          <t>6hKgCdFex2tTevTNokEmwovtGqtSYK2ps4AigmFwbonk</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -19343,7 +19343,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B245" t="n">
@@ -19351,7 +19351,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>2BLuupGDF6GWVJYZWB6fyJ75dWXjMzKGWVeN2TGppump</t>
+          <t>gkz69isayhx176GYZDE333gPyKoiAtMF2TGTNZwpump</t>
         </is>
       </c>
       <c r="F245" t="inlineStr">
@@ -19363,7 +19363,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B246" t="n">
@@ -19371,7 +19371,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>G114LVxZdHtsCfDuYjqP3u3RgmVTjKS6s8qHsHuKpump</t>
+          <t>8GRd7Eg6kFJZTvDdRQpRBX7w71s8R1wkQvMV3HWDT9PT</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -19383,7 +19383,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B247" t="n">
@@ -19391,7 +19391,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>B9z8cEWFmc7LvQtjKsaLoKqW5MJmGRCWqs1DPKupCfkk</t>
+          <t>FSyuCSheYUgtaSDa9iJVdVjgVf24XwipMLgWmjEbpump</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
@@ -19403,7 +19403,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B248" t="n">
@@ -19411,7 +19411,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>AYMwf7uvzTMnnDrw64zcMjLBGaqrVcSGP8eNKXtdpump</t>
+          <t>Dde3kgfE97FSCuYLpQHpJNLRcaFWXt6rnPcTc165pump</t>
         </is>
       </c>
       <c r="F248" t="inlineStr">
@@ -19423,7 +19423,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B249" t="n">
@@ -19431,7 +19431,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>4NWHUsqene63s56idLAchHC85MgvCucBgCsMjkiZpump</t>
+          <t>8PMg4GeyHCY1AWctg4ByowPSq35Pu9ZJHfNR4nAcbonk</t>
         </is>
       </c>
       <c r="F249" t="inlineStr">
@@ -19443,7 +19443,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B250" t="n">
@@ -19451,19 +19451,19 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
+          <t>3KuSj5VbdUCaSRXCXiUThNaJYjx4NPBbNNo4zmKzpump</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>Fallback:Master</t>
+          <t>DexProfilesLatest</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="B251" t="n">
@@ -19471,12 +19471,12 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
+          <t>8RwSa8i6sVhdU4KmXatE6syDgSDUEmKiZC6C4KCTpump</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>Fallback:Master</t>
+          <t>DexProfilesLatest</t>
         </is>
       </c>
     </row>
@@ -19554,12 +19554,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2FSn3q2gFFLvmsV4njXRc3z9ig9ypwY6TFVcBLLepump</t>
+          <t>2Mk8vAfersJgfeT5Pwpfe7y4sQ769GZPhRrnwSdhpump</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -19572,12 +19572,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Nzn8vsoshVehdiWbvBvgeTL3M1yWNhz1DF8A2AXLV7y</t>
+          <t>BuTM2tXzmuM6TcS9cTQhL1VaxjDfYtSHgKHkYQsFpRsX</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -19590,12 +19590,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EaEVXxVALRvgD3zFcsXZYkz4WTiCWBfpmakXwddDLive</t>
+          <t>BqndqeBCNSEftBKmbTbLVx1RX5zd5J3AGL9sG55Jpump</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -19608,12 +19608,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BDRLQzYHn7pypXWwg2zFXy4as5Km28iSTruGJxuQpump</t>
+          <t>6NdUMfsuyGENe98VPVMRxNZnbQgTUaKxLuiLszS5pump</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -19626,12 +19626,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>6V4QLouv2HTbae34hBjLgW5Qc3kdquqFLBsDS3scR1CH</t>
+          <t>oxynABVJXUEc9PLNx4m1XVdiFtRhStzRXG1G6qosni1</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -19644,12 +19644,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>q29umWshmh2fmm1CdRb4cBKhqtW9xX25ezNQi7Bpump</t>
+          <t>EMg2QkFZ6pLvgckVGj8X6nmyrkiuoamYnTdoxXN8pump</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -19662,12 +19662,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>C93Xk7zeJEYwqmWeJJCnWVsSR3Nog7SC7LHW2ZTxvREV</t>
+          <t>AufjSxXopMZn7EeX21ifncGPKQ2BH6FaiRpFu6gDpump</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -19680,12 +19680,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4KUCN58TeExp9qrap64yuBPTmGmToV7R9h1p7HCZpump</t>
+          <t>HBukB9DLbdTM6nNHQQ6JvVmjx7UmuMpDJAU9oX8tpump</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -19698,12 +19698,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>34AeqX5MQGyrey2VnZdkeZCfM4qinp4F3X7pGxtipump</t>
+          <t>xxxgjrRmEtAeik3fpkftHA6ncHjfDWWN4T1zUYQPm3z</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -19716,12 +19716,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3sLSDYfmbu5ZdmC7wbBUzvwRFE6S1dtrTUafuhhApump</t>
+          <t>2t2sKsaGpRG3jWV22y9eAVp7qfRRaytDiS1kkMpCqREV</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -19734,12 +19734,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>9DVgoPhCJkmS9C1tVCRyz4Ectu5MNsph9nwiQZAPmoon</t>
+          <t>DiiTPZdpd9t3XorHiuZUu4E1FoSaQ7uGN4q9YkQupump</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-19</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -19752,12 +19752,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
+          <t>CKVZPWFPaJArEaPnk16CXpFtFXjuCxCh95vBcS3Ppump</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -19770,12 +19770,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>A8YHuvQBMAxXoZAZE72FyC8B7jKHo8RJyByXRRffpump</t>
+          <t>UbNX69Ng8TiE84rc5x4aLY6mcmbPbyZ2BJ2nfhupump</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -19788,12 +19788,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>4NGbC4RRrUjS78ooSN53Up7gSg4dGrj6F6dxpMWHbonk</t>
+          <t>6NqgJiWQLVznisyn1ytHEtQkC52sQf4t1b732Qvvpump</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -19806,12 +19806,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>31ovHdpQJTMrmxwiSRWpZQ6oY3AP9wu8RWZh8adepump</t>
+          <t>EfFvS8CXAJ89Y3hP8cMpmtW1kDWTg4PnhLMkrW29pump</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -19824,12 +19824,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
+          <t>3d3suDtLDqnXyA454EYCkAnhz33P55FAMCEk37Gppump</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>2025-09-19</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -19842,12 +19842,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CB9dDufT3ZuQXqqSfa1c5kY935TEreyBw9XJXxHKpump</t>
+          <t>FjXD9UWJaG6iVhExBR9SC6HjPmFA3czPGLeSbxurpump</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -19860,12 +19860,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BVvywU1wt4FaLDfZe7y11yrVnHbJpAU7YirmsuW3pump</t>
+          <t>irSdJ3vRioPxMmN3ZFrG6Y7ECJtyyJBnUcLKMauA6tR</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -19878,12 +19878,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3rSKhRtrjHnSZhRsgoAtrWRVM8rcf8DYv8Quea1epump</t>
+          <t>919MM61rJb1KairDkbNoH8iCVkX1fGFn7w4Dj6Mapump</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -19896,12 +19896,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BPcEmH1Amv1ZAJhBpTxnTpkMg1bbkbrM7RwKycWipump</t>
+          <t>GEHJx1yb83BDdjWp6UJWWann9aAkVKwvzU49Qp7jpump</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -19914,12 +19914,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>HGwdb6RQsMTqXpjBiy5BEAXHcpanmJr3c1Dj84r5pump</t>
+          <t>4Ds7cxJ82gm34gV22zo2LjPdX3nFbQk9PXK7mjX4pump</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -19932,12 +19932,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>wCtiCRJz69a5Mqkk2nHmvQwBGQCrUvM8fELoFGqpump</t>
+          <t>3d1qHSAkQhoN7kN1C6tvpAArCkXWxwYdBng6taXCDM6u</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -19950,12 +19950,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>41m33JPaG3qGJjkJY1uMpLCiNXccaNxSm1wJyYjQ2LPR</t>
+          <t>CWVuqZzGfrXD5i1dJYyvpLaQW6yzPqaPC7UemZFUpump</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -19968,12 +19968,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>H9iZggMWYP8G6DxKRaDoRW8ZkE4miWVuqpKYLrAspump</t>
+          <t>8MWLo9PmNiunLFhCZsXBsHqmvKrxTjt3qffFJF81pump</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -19986,12 +19986,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BdDB5AH7azG8BQGC9bSobh6ER33VdB7ZZ97jGn2Npump</t>
+          <t>GaPbGp23pPuY9QBLPUjUEBn2MKEroTe9Q3M3f2Xpump</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -20004,12 +20004,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>AjgSvYmJLhvt3FteiyTqQf8XBj1SVs6T6AmSUfkHpump</t>
+          <t>7UgmCpkZMMQBUajCfhrtiJXZ1wPuMidEB4DnA6aUpump</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -20022,12 +20022,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5t3TrtpDm1P8pRVYXcJ6MmngNsv2Ty3H5cimDve2pump</t>
+          <t>5YesRCpnjAR396xDy1xenHahfogjevCH4c46TH6wPray</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -20040,12 +20040,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BoPBfkKgWGSDApzBjLi1RPwxvSoiN4ECTSPBH2qFpump</t>
+          <t>A6ec7AMvx7oH96sNYELiF5i3vw3YxCuN6Qb8fDMMpump</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -20058,12 +20058,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3SfAaAK5eFx4Q23VySQq35AESmHQoBjVJnG2CrXbpump</t>
+          <t>34wfgAa6JzKxN1TGCneRk3LY1xetvnF8q5n6H7fzf2TY</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H30" t="n">
@@ -20076,12 +20076,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CMHHKQAvfQZWEtxgWqLmhwrCqzzYikZqbTWPkEcCpump</t>
+          <t>ByC7sCHFL4s96JnwhbnC27dyY9iTzsjYDvx3XGgopump</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H31" t="n">
@@ -20094,12 +20094,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>xmcjcN35cwPheUALX7v3fczpJcCtAtZ2jgPPJkNYUFA</t>
+          <t>CWdRtpnFWVgTASioj6ZWPwca3j7i3Ya1hPF4QVL6bonk</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H32" t="n">
@@ -20112,12 +20112,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5BuA8VT8rfUM428FWThNNPE9MYYoZvv7ZtL89dB3pump</t>
+          <t>AS5DW5dHY9V46Mrz3VJAA2MsewkahDnHvv9tzNcnpump</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H33" t="n">
@@ -20130,12 +20130,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>J5FsJhyV5HTneY9PP4J6fkhiNnQaNQ4BzH4hAbDqeRNL</t>
+          <t>G9mRRd16qLYzbp7trdj7DFSZyLePM9DepaWnJJLwCUDF</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -20148,12 +20148,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>9FWysHuSHNrQnyJoC7qMbm2cLxjT9ttjqBKFp8tzpump</t>
+          <t>879iULwrP3VoPF7Ce2yxkMagpwecQLKkNtsY7DJrpump</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H35" t="n">
@@ -20166,12 +20166,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GWJcHRz6EZ2igjXfSWc7cz7PaJHfu8yMu4SL2Jqxpump</t>
+          <t>62GnkrYtLJBXoQWsCBHZVugkCDZzpBonAWX6CHmSpump</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H36" t="n">
@@ -20184,12 +20184,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CBhmj8ZUTMwDmWatE5Y3QHVzo3C5UXNpDg8YcGJMpump</t>
+          <t>3H9TNBGGh3jdBC76VdTJCB5QSSsKBKFnhM7164VnjpkM</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H37" t="n">
@@ -20202,12 +20202,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>EWdgTzAvBZwchg89f8CaJvtvc1dVish2Fa38jPGgpump</t>
+          <t>BSmKbyHpyWVamsGv6Ja7xEqAyMwNn4TRsyX4hFxEpump</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H38" t="n">
@@ -20220,12 +20220,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6ChfYhYQqZ2AfQbf4NMJUqJFGoNa26Y92hS7Ao9mpump</t>
+          <t>C8aogMqASuurkwKDzd6VZPNRqUTbVoDJH7GMiRYUpump</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H39" t="n">
@@ -20238,12 +20238,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CDzCp6fTS7K9pYZ1JEDb4ZpQ4B85BTqke9Kcmwpp5q3S</t>
+          <t>DrJnnTuBDLRZTQmtKgcBkFH3taLbGCNh9DBhWMkhpump</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H40" t="n">
@@ -20256,12 +20256,12 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>DD8TeSw8y7Q2D8MKSt47cTbAnAcHTFs6viov48PMFQQG</t>
+          <t>4uVEktQLeYdZHKVJP5FXzZLnzetwhfeyP8vyKXurpump</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H41" t="n">
@@ -20274,12 +20274,12 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>EpWd13A6dwnE8a4KEQx8XPDtaj7qViKZhhDCkmB7pump</t>
+          <t>8oCqyRtFXjYbeC7fhxQMAqu6eAMEoibjyJCQcLnopump</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H42" t="n">
@@ -20292,12 +20292,12 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2ps5iWYb4PW353wiGKb36EmieYGQKnBFjxEueenu2bPw</t>
+          <t>APbFhZNhR4goT1JbCFiTrw2N5rPckj5kWZLVzRtnBWLc</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H43" t="n">
@@ -20310,12 +20310,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>G9c3H8Hed4ZNnXvw2t9P1uJeXcQDmdn57Qi5UtGGpump</t>
+          <t>6hKgCdFex2tTevTNokEmwovtGqtSYK2ps4AigmFwbonk</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H44" t="n">
@@ -20328,12 +20328,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2BLuupGDF6GWVJYZWB6fyJ75dWXjMzKGWVeN2TGppump</t>
+          <t>gkz69isayhx176GYZDE333gPyKoiAtMF2TGTNZwpump</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H45" t="n">
@@ -20346,12 +20346,12 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>G114LVxZdHtsCfDuYjqP3u3RgmVTjKS6s8qHsHuKpump</t>
+          <t>8GRd7Eg6kFJZTvDdRQpRBX7w71s8R1wkQvMV3HWDT9PT</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H46" t="n">
@@ -20364,12 +20364,12 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>B9z8cEWFmc7LvQtjKsaLoKqW5MJmGRCWqs1DPKupCfkk</t>
+          <t>FSyuCSheYUgtaSDa9iJVdVjgVf24XwipMLgWmjEbpump</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H47" t="n">
@@ -20382,12 +20382,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>AYMwf7uvzTMnnDrw64zcMjLBGaqrVcSGP8eNKXtdpump</t>
+          <t>Dde3kgfE97FSCuYLpQHpJNLRcaFWXt6rnPcTc165pump</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H48" t="n">
@@ -20400,12 +20400,12 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>4NWHUsqene63s56idLAchHC85MgvCucBgCsMjkiZpump</t>
+          <t>8PMg4GeyHCY1AWctg4ByowPSq35Pu9ZJHfNR4nAcbonk</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H49" t="n">
@@ -20418,12 +20418,12 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
+          <t>3KuSj5VbdUCaSRXCXiUThNaJYjx4NPBbNNo4zmKzpump</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H50" t="n">
@@ -20436,12 +20436,12 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
+          <t>8RwSa8i6sVhdU4KmXatE6syDgSDUEmKiZC6C4KCTpump</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>2025-09-24</t>
+          <t>2025-09-26</t>
         </is>
       </c>
       <c r="H51" t="n">
@@ -20569,7 +20569,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-09-24T12:29:00.461557</t>
+          <t>2025-09-26T07:39:24.205222</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">

</xml_diff>

<commit_message>
chore: update reports (2025-09-27)
</commit_message>
<xml_diff>
--- a/sol_master_LIVE.xlsx
+++ b/sol_master_LIVE.xlsx
@@ -495,7 +495,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4.558875835164439e-06</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -527,14 +527,14 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -553,16 +553,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.862e-05</v>
+        <v>1.902e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>1085.21</v>
+        <v>677.04</v>
       </c>
       <c r="G3" t="n">
-        <v>24352.04</v>
+        <v>24974</v>
       </c>
       <c r="H3" t="n">
-        <v>18627</v>
+        <v>19022</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -573,7 +573,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -592,27 +592,27 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>6.836423046302206e-06</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>19.89</v>
+        <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>1923.56</v>
+        <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>6723</v>
+        <v>0</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -631,27 +631,27 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>4.353e-06</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>10.56</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>8409.379999999999</v>
+        <v>0</v>
       </c>
       <c r="H5" t="n">
-        <v>4352</v>
+        <v>0</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>dexscreener</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -670,27 +670,27 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>7.361831910819658e-06</v>
+        <v>7.866999999999999e-06</v>
       </c>
       <c r="F6" t="n">
-        <v>90.34</v>
+        <v>226.54</v>
       </c>
       <c r="G6" t="n">
-        <v>10174.38</v>
+        <v>10782.26</v>
       </c>
       <c r="H6" t="n">
-        <v>7357</v>
+        <v>7864</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -709,16 +709,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5.844e-06</v>
+        <v>6.564e-06</v>
       </c>
       <c r="F7" t="n">
-        <v>607.9299999999999</v>
+        <v>784.97</v>
       </c>
       <c r="G7" t="n">
-        <v>9226.719999999999</v>
+        <v>10080.12</v>
       </c>
       <c r="H7" t="n">
-        <v>5845</v>
+        <v>6564</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -729,7 +729,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -748,27 +748,27 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>8.696337810615279e-05</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.07000000000000001</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>3955</v>
+        <v>0</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -787,16 +787,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.00343</v>
+        <v>0.003726</v>
       </c>
       <c r="F9" t="n">
-        <v>11811.92</v>
+        <v>14194.93</v>
       </c>
       <c r="G9" t="n">
-        <v>506141.89</v>
+        <v>537626.26</v>
       </c>
       <c r="H9" t="n">
-        <v>3430724</v>
+        <v>3726039</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -807,7 +807,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -826,27 +826,27 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.0151740042472802</v>
+        <v>0.01555</v>
       </c>
       <c r="F10" t="n">
-        <v>90743.88</v>
+        <v>50695.03</v>
       </c>
       <c r="G10" t="n">
-        <v>1924904.53</v>
+        <v>1989078.44</v>
       </c>
       <c r="H10" t="n">
-        <v>75607327</v>
+        <v>77798794</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -865,16 +865,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.0005505</v>
+        <v>0.0004736</v>
       </c>
       <c r="F11" t="n">
-        <v>6313.41</v>
+        <v>8526.07</v>
       </c>
       <c r="G11" t="n">
-        <v>87938.64</v>
+        <v>82711.64</v>
       </c>
       <c r="H11" t="n">
-        <v>393147</v>
+        <v>338214</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -885,7 +885,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -904,27 +904,27 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>7.593580296311352e-06</v>
+        <v>8.111000000000001e-06</v>
       </c>
       <c r="F12" t="n">
-        <v>443.43</v>
+        <v>376.17</v>
       </c>
       <c r="G12" t="n">
-        <v>5738.96</v>
+        <v>5714.17</v>
       </c>
       <c r="H12" t="n">
-        <v>8475</v>
+        <v>8112</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -943,16 +943,16 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.11e-05</v>
+        <v>8.765e-06</v>
       </c>
       <c r="F13" t="n">
-        <v>5367.66</v>
+        <v>4772.9</v>
       </c>
       <c r="G13" t="n">
-        <v>13646.44</v>
+        <v>12334.21</v>
       </c>
       <c r="H13" t="n">
-        <v>11104</v>
+        <v>8762</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -963,7 +963,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -982,27 +982,27 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>4.583838996334617e-05</v>
+        <v>4.887e-05</v>
       </c>
       <c r="F14" t="n">
-        <v>13684.01</v>
+        <v>23841.19</v>
       </c>
       <c r="G14" t="n">
-        <v>30401.16</v>
+        <v>28863.09</v>
       </c>
       <c r="H14" t="n">
-        <v>54967</v>
+        <v>48878</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1021,27 +1021,27 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>6.556e-06</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>338.45</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>9872.629999999999</v>
+        <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>6040</v>
+        <v>0</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>dexscreener</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1060,27 +1060,27 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2.669227773281133e-05</v>
+        <v>3.199e-05</v>
       </c>
       <c r="F16" t="n">
-        <v>9418.15</v>
+        <v>3394.76</v>
       </c>
       <c r="G16" t="n">
-        <v>19956.76</v>
+        <v>22140.32</v>
       </c>
       <c r="H16" t="n">
-        <v>26669</v>
+        <v>31993</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1099,16 +1099,16 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2.467e-05</v>
+        <v>2.771e-05</v>
       </c>
       <c r="F17" t="n">
-        <v>4437.35</v>
+        <v>3064.45</v>
       </c>
       <c r="G17" t="n">
-        <v>22401.27</v>
+        <v>24165.35</v>
       </c>
       <c r="H17" t="n">
-        <v>24668</v>
+        <v>27715</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1119,7 +1119,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1138,27 +1138,27 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.628157003570316e-05</v>
+        <v>1.315e-05</v>
       </c>
       <c r="F18" t="n">
-        <v>38138.11</v>
+        <v>4511.17</v>
       </c>
       <c r="G18" t="n">
-        <v>17045.46</v>
+        <v>15481.35</v>
       </c>
       <c r="H18" t="n">
-        <v>16502</v>
+        <v>13150</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1177,16 +1177,16 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.002227</v>
+        <v>0.002219</v>
       </c>
       <c r="F19" t="n">
-        <v>89459.37</v>
+        <v>74296.28</v>
       </c>
       <c r="G19" t="n">
-        <v>198388.12</v>
+        <v>201654.09</v>
       </c>
       <c r="H19" t="n">
-        <v>2227455</v>
+        <v>2219839</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1197,7 +1197,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1216,27 +1216,27 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.001451470253266603</v>
+        <v>0.001564</v>
       </c>
       <c r="F20" t="n">
-        <v>157597.64</v>
+        <v>166574.4</v>
       </c>
       <c r="G20" t="n">
-        <v>178245.8</v>
+        <v>188886.87</v>
       </c>
       <c r="H20" t="n">
-        <v>1449819</v>
+        <v>1563775</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1255,16 +1255,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.0004406</v>
+        <v>0.0004767</v>
       </c>
       <c r="F21" t="n">
-        <v>139092.77</v>
+        <v>149256.84</v>
       </c>
       <c r="G21" t="n">
-        <v>118204.19</v>
+        <v>125385.97</v>
       </c>
       <c r="H21" t="n">
-        <v>440573</v>
+        <v>476700</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1275,7 +1275,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1294,27 +1294,27 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.002214253718620511</v>
+        <v>0.002063</v>
       </c>
       <c r="F22" t="n">
-        <v>6683461.67</v>
+        <v>1452578.39</v>
       </c>
       <c r="G22" t="n">
-        <v>237475.42</v>
+        <v>236056.27</v>
       </c>
       <c r="H22" t="n">
-        <v>1715862</v>
+        <v>1603514</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1333,16 +1333,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1.623e-05</v>
+        <v>1.362e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>2553.93</v>
+        <v>1252.56</v>
       </c>
       <c r="G23" t="n">
-        <v>17600.77</v>
+        <v>16329.19</v>
       </c>
       <c r="H23" t="n">
-        <v>15953</v>
+        <v>13381</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1353,7 +1353,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1372,27 +1372,27 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1.505544749935503e-06</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>20.7</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>2738.48</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>1528</v>
+        <v>0</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1411,16 +1411,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.0008863</v>
+        <v>0.0007838</v>
       </c>
       <c r="F25" t="n">
-        <v>189897.46</v>
+        <v>120914.05</v>
       </c>
       <c r="G25" t="n">
-        <v>189828.63</v>
+        <v>181844.76</v>
       </c>
       <c r="H25" t="n">
-        <v>886307</v>
+        <v>783870</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1431,7 +1431,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1450,27 +1450,27 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>3.649919466916757e-06</v>
+        <v>0</v>
       </c>
       <c r="F26" t="n">
-        <v>117.76</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>7149.44</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>3646</v>
+        <v>0</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1489,16 +1489,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>9.613e-05</v>
+        <v>0.0001214</v>
       </c>
       <c r="F27" t="n">
-        <v>14335.39</v>
+        <v>13882.23</v>
       </c>
       <c r="G27" t="n">
-        <v>47273.98</v>
+        <v>54055.4</v>
       </c>
       <c r="H27" t="n">
-        <v>96089</v>
+        <v>121363</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1509,7 +1509,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1528,27 +1528,27 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>5.546854970348866e-06</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>0.6899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G28" t="n">
         <v>0</v>
       </c>
       <c r="H28" t="n">
-        <v>5543.11</v>
+        <v>0</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1587,7 +1587,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1606,27 +1606,27 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>5.586094122672058e-06</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.39</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
         <v>0</v>
       </c>
       <c r="H30" t="n">
-        <v>5585.2</v>
+        <v>0</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1645,27 +1645,27 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>4.087e-06</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>68.26000000000001</v>
+        <v>0</v>
       </c>
       <c r="G31" t="n">
-        <v>7588.53</v>
+        <v>0</v>
       </c>
       <c r="H31" t="n">
-        <v>4081</v>
+        <v>0</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>dexscreener</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1684,27 +1684,27 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.111372346912996</v>
+        <v>1.15</v>
       </c>
       <c r="F32" t="n">
-        <v>1587329.8</v>
+        <v>148.72</v>
       </c>
       <c r="G32" t="n">
-        <v>2502580.03</v>
+        <v>2603982.57</v>
       </c>
       <c r="H32" t="n">
-        <v>23334274</v>
+        <v>24232529</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1743,7 +1743,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1762,7 +1762,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>5.997298052119634e-06</v>
+        <v>0</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1775,14 +1775,14 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1821,7 +1821,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1840,7 +1840,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>6.130100405371453e-06</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1853,14 +1853,14 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1879,16 +1879,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1.799e-05</v>
+        <v>1.825e-05</v>
       </c>
       <c r="F37" t="n">
-        <v>6313.01</v>
+        <v>3468.94</v>
       </c>
       <c r="G37" t="n">
-        <v>16500.7</v>
+        <v>16887.13</v>
       </c>
       <c r="H37" t="n">
-        <v>17896</v>
+        <v>18158</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -1899,7 +1899,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1918,7 +1918,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>6.219203669339925e-06</v>
+        <v>0</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1931,14 +1931,14 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1977,7 +1977,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1996,7 +1996,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>6.020951632771035e-06</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -2009,14 +2009,14 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>birdeye</t>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2055,7 +2055,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2074,27 +2074,27 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>5.54450923731753e-06</v>
+        <v>5.68e-06</v>
       </c>
       <c r="F42" t="n">
-        <v>4.02</v>
+        <v>17.3</v>
       </c>
       <c r="G42" t="n">
-        <v>8660.870000000001</v>
+        <v>9036.16</v>
       </c>
       <c r="H42" t="n">
-        <v>5463</v>
+        <v>5678</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2113,16 +2113,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>4.406e-05</v>
+        <v>3.924e-05</v>
       </c>
       <c r="F43" t="n">
-        <v>11897.48</v>
+        <v>6888.29</v>
       </c>
       <c r="G43" t="n">
-        <v>27293.03</v>
+        <v>26239.13</v>
       </c>
       <c r="H43" t="n">
-        <v>44067</v>
+        <v>39242</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2133,7 +2133,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2152,27 +2152,27 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>5.977165642249016e-06</v>
+        <v>6.142e-06</v>
       </c>
       <c r="F44" t="n">
-        <v>0.79</v>
+        <v>1.31</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>5975.02</v>
+        <v>6142.25</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2191,16 +2191,16 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3.72e-06</v>
+        <v>3.886e-06</v>
       </c>
       <c r="F45" t="n">
-        <v>10.66</v>
+        <v>6.25</v>
       </c>
       <c r="G45" t="n">
-        <v>7134.75</v>
+        <v>7466.77</v>
       </c>
       <c r="H45" t="n">
-        <v>3718</v>
+        <v>3884</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2211,7 +2211,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2230,27 +2230,27 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3.400529426019206e-05</v>
+        <v>3.057e-05</v>
       </c>
       <c r="F46" t="n">
-        <v>9736.51</v>
+        <v>2793.7</v>
       </c>
       <c r="G46" t="n">
-        <v>21632.46</v>
+        <v>20937.82</v>
       </c>
       <c r="H46" t="n">
-        <v>33987</v>
+        <v>30575</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2269,16 +2269,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>4.552e-06</v>
+        <v>4.901e-06</v>
       </c>
       <c r="F47" t="n">
-        <v>18.63</v>
+        <v>100.29</v>
       </c>
       <c r="G47" t="n">
-        <v>8001.79</v>
+        <v>8409.16</v>
       </c>
       <c r="H47" t="n">
-        <v>4552</v>
+        <v>4901</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2289,7 +2289,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2308,27 +2308,27 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5.453612762251914e-06</v>
+        <v>5.51e-06</v>
       </c>
       <c r="F48" t="n">
-        <v>27.78</v>
+        <v>52.08</v>
       </c>
       <c r="G48" t="n">
-        <v>8862</v>
+        <v>9027.700000000001</v>
       </c>
       <c r="H48" t="n">
-        <v>5447</v>
+        <v>5507</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2347,27 +2347,27 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>5.311969760914955e-06</v>
+        <v>5.551e-06</v>
       </c>
       <c r="F49" t="n">
-        <v>160.63</v>
+        <v>259.26</v>
       </c>
       <c r="G49" t="n">
-        <v>8496.57</v>
+        <v>8933.969999999999</v>
       </c>
       <c r="H49" t="n">
-        <v>5305</v>
+        <v>5548</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2386,16 +2386,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>4.594e-06</v>
+        <v>4.762e-06</v>
       </c>
       <c r="F50" t="n">
-        <v>10.89</v>
+        <v>0.11</v>
       </c>
       <c r="G50" t="n">
-        <v>8504.620000000001</v>
+        <v>8815.77</v>
       </c>
       <c r="H50" t="n">
-        <v>4594</v>
+        <v>4762</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -2406,7 +2406,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-09-26</t>
+          <t>2025-09-27</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2425,20 +2425,20 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>5.304346326630492e-06</v>
+        <v>5.45e-06</v>
       </c>
       <c r="F51" t="n">
-        <v>9.94</v>
+        <v>0.15</v>
       </c>
       <c r="G51" t="n">
-        <v>10132.37</v>
+        <v>10424.01</v>
       </c>
       <c r="H51" t="n">
-        <v>5299</v>
+        <v>5448</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>dexscreener+birdeye</t>
+          <t>dexscreener</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: update reports (2025-09-28)
</commit_message>
<xml_diff>
--- a/sol_master_LIVE.xlsx
+++ b/sol_master_LIVE.xlsx
@@ -505,7 +505,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -552,7 +552,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>1.91e-05</v>
+        <v>1.826e-05</v>
       </c>
       <c r="F3" t="n">
-        <v>285.32</v>
+        <v>283.83</v>
       </c>
       <c r="G3" t="n">
-        <v>25043.61</v>
+        <v>24436.1</v>
       </c>
       <c r="H3" t="n">
-        <v>19104</v>
+        <v>18266</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -599,7 +599,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -646,7 +646,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -693,7 +693,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -712,16 +712,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>7.847e-06</v>
+        <v>7.776e-06</v>
       </c>
       <c r="F6" t="n">
-        <v>230.9</v>
+        <v>11.81</v>
       </c>
       <c r="G6" t="n">
-        <v>10758.08</v>
+        <v>10734.17</v>
       </c>
       <c r="H6" t="n">
-        <v>7844</v>
+        <v>7773</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -740,7 +740,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -759,16 +759,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>6.119e-06</v>
+        <v>6.166e-06</v>
       </c>
       <c r="F7" t="n">
-        <v>381.75</v>
+        <v>152.21</v>
       </c>
       <c r="G7" t="n">
-        <v>9677.5</v>
+        <v>9758.469999999999</v>
       </c>
       <c r="H7" t="n">
-        <v>6119</v>
+        <v>6167</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -834,7 +834,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -853,16 +853,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.003749</v>
+        <v>0.003768</v>
       </c>
       <c r="F9" t="n">
-        <v>14477.15</v>
+        <v>7388.42</v>
       </c>
       <c r="G9" t="n">
-        <v>539354.4300000001</v>
+        <v>539325.08</v>
       </c>
       <c r="H9" t="n">
-        <v>3749359</v>
+        <v>3768217</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -881,7 +881,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -900,16 +900,16 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.01548</v>
+        <v>0.01528</v>
       </c>
       <c r="F10" t="n">
-        <v>45159.33</v>
+        <v>12797.21</v>
       </c>
       <c r="G10" t="n">
-        <v>1984584.19</v>
+        <v>1959646.06</v>
       </c>
       <c r="H10" t="n">
-        <v>77435322</v>
+        <v>76409647</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -947,16 +947,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.0004504</v>
+        <v>0.0004327</v>
       </c>
       <c r="F11" t="n">
-        <v>7909.81</v>
+        <v>2108.61</v>
       </c>
       <c r="G11" t="n">
-        <v>80799.14</v>
+        <v>78771.32000000001</v>
       </c>
       <c r="H11" t="n">
-        <v>321675</v>
+        <v>309020</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -975,7 +975,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -994,16 +994,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>8.094000000000001e-06</v>
+        <v>5.216e-06</v>
       </c>
       <c r="F12" t="n">
-        <v>612.83</v>
+        <v>1177.07</v>
       </c>
       <c r="G12" t="n">
-        <v>5716.02</v>
+        <v>4591.41</v>
       </c>
       <c r="H12" t="n">
-        <v>8095</v>
+        <v>5216</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1041,16 +1041,16 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1.032e-05</v>
+        <v>7.762e-06</v>
       </c>
       <c r="F13" t="n">
-        <v>2975.67</v>
+        <v>2547.84</v>
       </c>
       <c r="G13" t="n">
-        <v>13374.02</v>
+        <v>11553.06</v>
       </c>
       <c r="H13" t="n">
-        <v>10317</v>
+        <v>7759</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1088,16 +1088,16 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>4.826e-05</v>
+        <v>4.95e-05</v>
       </c>
       <c r="F14" t="n">
-        <v>8491.57</v>
+        <v>8327.969999999999</v>
       </c>
       <c r="G14" t="n">
-        <v>28708.51</v>
+        <v>29049.01</v>
       </c>
       <c r="H14" t="n">
-        <v>48270</v>
+        <v>49503</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1116,7 +1116,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1163,7 +1163,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1182,16 +1182,16 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>3.092e-05</v>
+        <v>2.98e-05</v>
       </c>
       <c r="F16" t="n">
-        <v>2944.06</v>
+        <v>891.04</v>
       </c>
       <c r="G16" t="n">
-        <v>21795.37</v>
+        <v>21340.56</v>
       </c>
       <c r="H16" t="n">
-        <v>30926</v>
+        <v>29808</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1229,16 +1229,16 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>2.979e-05</v>
+        <v>2.644e-05</v>
       </c>
       <c r="F17" t="n">
-        <v>2595.08</v>
+        <v>1869.97</v>
       </c>
       <c r="G17" t="n">
-        <v>25072.56</v>
+        <v>23493.4</v>
       </c>
       <c r="H17" t="n">
-        <v>29789</v>
+        <v>26442</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1276,16 +1276,16 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>1.334e-05</v>
+        <v>1.245e-05</v>
       </c>
       <c r="F18" t="n">
-        <v>8403.99</v>
+        <v>7554.03</v>
       </c>
       <c r="G18" t="n">
-        <v>15613.15</v>
+        <v>15005</v>
       </c>
       <c r="H18" t="n">
-        <v>13347</v>
+        <v>12455</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1304,7 +1304,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1323,16 +1323,16 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.002165</v>
+        <v>0.001994</v>
       </c>
       <c r="F19" t="n">
-        <v>54874.03</v>
+        <v>35091.84</v>
       </c>
       <c r="G19" t="n">
-        <v>199407.33</v>
+        <v>190581.55</v>
       </c>
       <c r="H19" t="n">
-        <v>2165020</v>
+        <v>1994992</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1370,16 +1370,16 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.001507</v>
+        <v>0.00137</v>
       </c>
       <c r="F20" t="n">
-        <v>116236.85</v>
+        <v>69006.14999999999</v>
       </c>
       <c r="G20" t="n">
-        <v>185690.09</v>
+        <v>176169.18</v>
       </c>
       <c r="H20" t="n">
-        <v>1507679</v>
+        <v>1369922</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1398,7 +1398,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1417,16 +1417,16 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.0004706</v>
+        <v>0.0004403</v>
       </c>
       <c r="F21" t="n">
-        <v>148055.68</v>
+        <v>93739.56</v>
       </c>
       <c r="G21" t="n">
-        <v>124623.89</v>
+        <v>120150.22</v>
       </c>
       <c r="H21" t="n">
-        <v>470575</v>
+        <v>440268</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1445,7 +1445,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1464,16 +1464,16 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.001793</v>
+        <v>0.001543</v>
       </c>
       <c r="F22" t="n">
-        <v>1302307.25</v>
+        <v>792802.78</v>
       </c>
       <c r="G22" t="n">
-        <v>220653.01</v>
+        <v>205059.58</v>
       </c>
       <c r="H22" t="n">
-        <v>1393574</v>
+        <v>1199692</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1492,7 +1492,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1511,16 +1511,16 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>1.349e-05</v>
+        <v>1.541e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>1228.65</v>
+        <v>726.77</v>
       </c>
       <c r="G23" t="n">
-        <v>16268.16</v>
+        <v>17293.73</v>
       </c>
       <c r="H23" t="n">
-        <v>13253</v>
+        <v>15148</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1586,7 +1586,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1605,16 +1605,16 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.0007527</v>
+        <v>0.0007231</v>
       </c>
       <c r="F25" t="n">
-        <v>93663.34</v>
+        <v>61989.1</v>
       </c>
       <c r="G25" t="n">
-        <v>178403.94</v>
+        <v>174071.69</v>
       </c>
       <c r="H25" t="n">
-        <v>752703</v>
+        <v>723103</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1680,7 +1680,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1699,16 +1699,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.0001293</v>
+        <v>0.0001181</v>
       </c>
       <c r="F27" t="n">
-        <v>8314.889999999999</v>
+        <v>13738.92</v>
       </c>
       <c r="G27" t="n">
-        <v>55861.6</v>
+        <v>53336.84</v>
       </c>
       <c r="H27" t="n">
-        <v>129242</v>
+        <v>118069</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1727,7 +1727,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1774,7 +1774,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1821,7 +1821,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1868,7 +1868,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1915,7 +1915,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1934,16 +1934,16 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>1.16</v>
+        <v>1.14</v>
       </c>
       <c r="F32" t="n">
-        <v>139.13</v>
+        <v>629.65</v>
       </c>
       <c r="G32" t="n">
-        <v>2638336.47</v>
+        <v>2594056.05</v>
       </c>
       <c r="H32" t="n">
-        <v>24550708</v>
+        <v>24133304</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2009,7 +2009,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2056,7 +2056,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2103,7 +2103,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2150,7 +2150,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2169,16 +2169,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>1.893e-05</v>
+        <v>1.701e-05</v>
       </c>
       <c r="F37" t="n">
-        <v>2336.62</v>
+        <v>1335.83</v>
       </c>
       <c r="G37" t="n">
-        <v>17244.39</v>
+        <v>16249.92</v>
       </c>
       <c r="H37" t="n">
-        <v>18837</v>
+        <v>16925</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2197,7 +2197,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2216,25 +2216,25 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>5.864e-06</v>
       </c>
       <c r="F38" t="n">
-        <v>0</v>
+        <v>4.95</v>
       </c>
       <c r="G38" t="n">
         <v>0</v>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>5864.93</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>none</t>
+          <t>dexscreener</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>missing</t>
+          <t>ok</t>
         </is>
       </c>
       <c r="K38" t="n">
@@ -2244,7 +2244,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2291,7 +2291,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2338,7 +2338,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2385,7 +2385,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2404,16 +2404,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>5.677e-06</v>
+        <v>5.735e-06</v>
       </c>
       <c r="F42" t="n">
-        <v>219.97</v>
+        <v>213.28</v>
       </c>
       <c r="G42" t="n">
-        <v>9022.209999999999</v>
+        <v>9065.77</v>
       </c>
       <c r="H42" t="n">
-        <v>5675</v>
+        <v>5733</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2451,16 +2451,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>3.639e-05</v>
+        <v>3.927e-05</v>
       </c>
       <c r="F43" t="n">
-        <v>6711.65</v>
+        <v>4270.63</v>
       </c>
       <c r="G43" t="n">
-        <v>25290.56</v>
+        <v>26131</v>
       </c>
       <c r="H43" t="n">
-        <v>36397</v>
+        <v>39270</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2479,7 +2479,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2498,25 +2498,25 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>6.142e-06</v>
+        <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>1.31</v>
+        <v>0</v>
       </c>
       <c r="G44" t="n">
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>6142.25</v>
+        <v>0</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>dexscreener</t>
+          <t>none</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>missing</t>
         </is>
       </c>
       <c r="K44" t="n">
@@ -2526,7 +2526,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2545,25 +2545,25 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>3.886e-06</v>
+        <v>0</v>
       </c>
       <c r="F45" t="n">
-        <v>6.25</v>
+        <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>7466.77</v>
+        <v>0</v>
       </c>
       <c r="H45" t="n">
-        <v>3884</v>
+        <v>0</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>dexscreener</t>
+          <t>none</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>missing</t>
         </is>
       </c>
       <c r="K45" t="n">
@@ -2573,7 +2573,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2592,16 +2592,16 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>3.048e-05</v>
+        <v>2.956e-05</v>
       </c>
       <c r="F46" t="n">
-        <v>2157.62</v>
+        <v>621.5700000000001</v>
       </c>
       <c r="G46" t="n">
-        <v>20919.23</v>
+        <v>20488.98</v>
       </c>
       <c r="H46" t="n">
-        <v>30483</v>
+        <v>29561</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -2620,7 +2620,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2639,16 +2639,16 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>4.93e-06</v>
+        <v>4.893e-06</v>
       </c>
       <c r="F47" t="n">
-        <v>101.27</v>
+        <v>7.37</v>
       </c>
       <c r="G47" t="n">
-        <v>8456.75</v>
+        <v>8398.870000000001</v>
       </c>
       <c r="H47" t="n">
-        <v>4931</v>
+        <v>4893</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2667,7 +2667,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2686,25 +2686,25 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5.51e-06</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="G48" t="n">
-        <v>9027.700000000001</v>
+        <v>0</v>
       </c>
       <c r="H48" t="n">
-        <v>5507</v>
+        <v>0</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>dexscreener</t>
+          <t>none</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>missing</t>
         </is>
       </c>
       <c r="K48" t="n">
@@ -2714,7 +2714,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2733,25 +2733,25 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>5.551e-06</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>237.84</v>
+        <v>0</v>
       </c>
       <c r="G49" t="n">
-        <v>8933.969999999999</v>
+        <v>0</v>
       </c>
       <c r="H49" t="n">
-        <v>5548</v>
+        <v>0</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>dexscreener</t>
+          <t>none</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>ok</t>
+          <t>missing</t>
         </is>
       </c>
       <c r="K49" t="n">
@@ -2761,7 +2761,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2780,16 +2780,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>4.7e-06</v>
+        <v>4.764e-06</v>
       </c>
       <c r="F50" t="n">
-        <v>0.8100000000000001</v>
+        <v>3.37</v>
       </c>
       <c r="G50" t="n">
-        <v>8700.27</v>
+        <v>8823.639999999999</v>
       </c>
       <c r="H50" t="n">
-        <v>4699</v>
+        <v>4763</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -2808,7 +2808,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-09-27</t>
+          <t>2025-09-28</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2827,16 +2827,16 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>5.496e-06</v>
+        <v>5.466e-06</v>
       </c>
       <c r="F51" t="n">
-        <v>0.15</v>
+        <v>0.27</v>
       </c>
       <c r="G51" t="n">
-        <v>10512.12</v>
+        <v>10454.08</v>
       </c>
       <c r="H51" t="n">
-        <v>5494</v>
+        <v>5464</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
chore: update reports (2025-09-29)
</commit_message>
<xml_diff>
--- a/sol_master_LIVE.xlsx
+++ b/sol_master_LIVE.xlsx
@@ -505,7 +505,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -524,13 +524,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>207.33</v>
+        <v>208.59</v>
       </c>
       <c r="F2" t="n">
-        <v>131062021.31</v>
+        <v>145041225.73</v>
       </c>
       <c r="G2" t="n">
-        <v>53758573.26</v>
+        <v>53724975.43</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -552,7 +552,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -571,16 +571,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.001608</v>
+        <v>0.001573</v>
       </c>
       <c r="F3" t="n">
-        <v>671185</v>
+        <v>552077.41</v>
       </c>
       <c r="G3" t="n">
-        <v>213678</v>
+        <v>212449.52</v>
       </c>
       <c r="H3" t="n">
-        <v>1250368</v>
+        <v>1222781</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -599,7 +599,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -618,16 +618,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.002652</v>
+        <v>0.002683</v>
       </c>
       <c r="F4" t="n">
-        <v>337560.81</v>
+        <v>313022.87</v>
       </c>
       <c r="G4" t="n">
-        <v>483698.31</v>
+        <v>488671.09</v>
       </c>
       <c r="H4" t="n">
-        <v>2651433</v>
+        <v>2681704</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -646,7 +646,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -665,16 +665,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.0007033</v>
+        <v>0.0005575000000000001</v>
       </c>
       <c r="F5" t="n">
-        <v>241693.96</v>
+        <v>185559.73</v>
       </c>
       <c r="G5" t="n">
-        <v>167930.48</v>
+        <v>150199.19</v>
       </c>
       <c r="H5" t="n">
-        <v>703233</v>
+        <v>557424</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -693,7 +693,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -708,20 +708,20 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CEqFiJoB6HLncfeieBw3PKKm9wyqrpSHV3VH4qZApump</t>
+          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.0005832</v>
+        <v>0.0004107</v>
       </c>
       <c r="F6" t="n">
-        <v>139841.69</v>
+        <v>154696.01</v>
       </c>
       <c r="G6" t="n">
-        <v>151467.95</v>
+        <v>118973.11</v>
       </c>
       <c r="H6" t="n">
-        <v>583233</v>
+        <v>410736</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -740,7 +740,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -755,20 +755,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CZkxnM5PNPak31JSFNzJ76CWcYRu4mgxvBwcHaBJpump</t>
+          <t>CEqFiJoB6HLncfeieBw3PKKm9wyqrpSHV3VH4qZApump</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.0004219</v>
+        <v>0.0004882</v>
       </c>
       <c r="F7" t="n">
-        <v>107391.27</v>
+        <v>144287.41</v>
       </c>
       <c r="G7" t="n">
-        <v>120011.08</v>
+        <v>139281.36</v>
       </c>
       <c r="H7" t="n">
-        <v>421889</v>
+        <v>488204</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -787,7 +787,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -806,16 +806,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.001317</v>
+        <v>0.001315</v>
       </c>
       <c r="F8" t="n">
-        <v>90504.58</v>
+        <v>142690.71</v>
       </c>
       <c r="G8" t="n">
-        <v>176068.08</v>
+        <v>176788.18</v>
       </c>
       <c r="H8" t="n">
-        <v>1317317</v>
+        <v>1315601</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -834,7 +834,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -849,20 +849,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>BVvSqvTb9ZVNEkP5UsamR1egAWSGEZiQDU42FS7mmoon</t>
+          <t>2UfyNHveDrYDogW1LypkworjhYVEte8tLDqRTZbguPLx</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.0004153</v>
+        <v>0.001819</v>
       </c>
       <c r="F9" t="n">
-        <v>78089.16</v>
+        <v>125795.2</v>
       </c>
       <c r="G9" t="n">
-        <v>92259.53999999999</v>
+        <v>202747.8</v>
       </c>
       <c r="H9" t="n">
-        <v>413964</v>
+        <v>1819061</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -881,7 +881,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -896,20 +896,20 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2UfyNHveDrYDogW1LypkworjhYVEte8tLDqRTZbguPLx</t>
+          <t>BVvSqvTb9ZVNEkP5UsamR1egAWSGEZiQDU42FS7mmoon</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.001629</v>
+        <v>0.0005583</v>
       </c>
       <c r="F10" t="n">
-        <v>75248.77</v>
+        <v>92276.99000000001</v>
       </c>
       <c r="G10" t="n">
-        <v>190774.71</v>
+        <v>105245.65</v>
       </c>
       <c r="H10" t="n">
-        <v>1629933</v>
+        <v>556466</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -947,16 +947,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.001859</v>
+        <v>0.001802</v>
       </c>
       <c r="F11" t="n">
-        <v>64579.14</v>
+        <v>83971.47</v>
       </c>
       <c r="G11" t="n">
-        <v>187418.09</v>
+        <v>185287.23</v>
       </c>
       <c r="H11" t="n">
-        <v>1859995</v>
+        <v>1802224</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -975,7 +975,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -994,16 +994,16 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.0007766</v>
+        <v>0.0008881</v>
       </c>
       <c r="F12" t="n">
-        <v>52950.14</v>
+        <v>79747.91</v>
       </c>
       <c r="G12" t="n">
-        <v>183874.6</v>
+        <v>197436.38</v>
       </c>
       <c r="H12" t="n">
-        <v>776639</v>
+        <v>888137</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1022,7 +1022,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1037,20 +1037,20 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>44DNPJ2qisA7MMaUmKK5SXvAcPyV7bEzmnK7oYJkbonk</t>
+          <t>2sjdF9vLNWkTpK2XgY2kVWCL4YTMu6vaVA4VxrzUpump</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.0001597</v>
+        <v>0.0001189</v>
       </c>
       <c r="F13" t="n">
-        <v>45360.26</v>
+        <v>48244.3</v>
       </c>
       <c r="G13" t="n">
-        <v>49491.33</v>
+        <v>57148.44</v>
       </c>
       <c r="H13" t="n">
-        <v>159742</v>
+        <v>118760</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1069,7 +1069,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1084,20 +1084,20 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
+          <t>44DNPJ2qisA7MMaUmKK5SXvAcPyV7bEzmnK7oYJkbonk</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>8.243e-05</v>
+        <v>0.0001899</v>
       </c>
       <c r="F14" t="n">
-        <v>38818.7</v>
+        <v>46254.95</v>
       </c>
       <c r="G14" t="n">
-        <v>42450.9</v>
+        <v>54033.63</v>
       </c>
       <c r="H14" t="n">
-        <v>82433</v>
+        <v>189928</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1116,7 +1116,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1131,20 +1131,20 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
+          <t>7ukFzJA7V6f28YieCjXcEXqiK8tAfbyXyvK6b36pump</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.0001508</v>
+        <v>0.0003006</v>
       </c>
       <c r="F15" t="n">
-        <v>27705.51</v>
+        <v>34688.03</v>
       </c>
       <c r="G15" t="n">
-        <v>52283.39</v>
+        <v>70932.71000000001</v>
       </c>
       <c r="H15" t="n">
-        <v>150892</v>
+        <v>300646</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1163,7 +1163,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1178,20 +1178,20 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>7kN5FQMD8ja4bzysEgc5FXmryKd6gCgjiWnhksjHCFb3</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.0001499</v>
+        <v>0.01561</v>
       </c>
       <c r="F16" t="n">
-        <v>23210.15</v>
+        <v>30869.5</v>
       </c>
       <c r="G16" t="n">
-        <v>55457.22</v>
+        <v>2028704.42</v>
       </c>
       <c r="H16" t="n">
-        <v>145463</v>
+        <v>78080891</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1210,7 +1210,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1225,20 +1225,20 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>7kN5FQMD8ja4bzysEgc5FXmryKd6gCgjiWnhksjHCFb3</t>
+          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.01565</v>
+        <v>9.123000000000001e-05</v>
       </c>
       <c r="F17" t="n">
-        <v>18786.54</v>
+        <v>28771.97</v>
       </c>
       <c r="G17" t="n">
-        <v>2021987.69</v>
+        <v>44882.57</v>
       </c>
       <c r="H17" t="n">
-        <v>78256305</v>
+        <v>91229</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
@@ -1257,7 +1257,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1272,20 +1272,20 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2sjdF9vLNWkTpK2XgY2kVWCL4YTMu6vaVA4VxrzUpump</t>
+          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.000106</v>
+        <v>0.0001402</v>
       </c>
       <c r="F18" t="n">
-        <v>17896.18</v>
+        <v>24955.71</v>
       </c>
       <c r="G18" t="n">
-        <v>53626.37</v>
+        <v>50653.6</v>
       </c>
       <c r="H18" t="n">
-        <v>105888</v>
+        <v>140227</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1304,7 +1304,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1319,20 +1319,20 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>6FtbGaqgZzti1TxJksBV4PSya5of9VqA9vJNDxPwbonk</t>
+          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.0005542</v>
+        <v>0.0001485</v>
       </c>
       <c r="F19" t="n">
-        <v>17048.81</v>
+        <v>23400.49</v>
       </c>
       <c r="G19" t="n">
-        <v>185358.39</v>
+        <v>55513.89</v>
       </c>
       <c r="H19" t="n">
-        <v>554249</v>
+        <v>144087</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1366,20 +1366,20 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>7ukFzJA7V6f28YieCjXcEXqiK8tAfbyXyvK6b36pump</t>
+          <t>6FtbGaqgZzti1TxJksBV4PSya5of9VqA9vJNDxPwbonk</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.0003053</v>
+        <v>0.0005196000000000001</v>
       </c>
       <c r="F20" t="n">
-        <v>12210.02</v>
+        <v>14611.99</v>
       </c>
       <c r="G20" t="n">
-        <v>71075.64999999999</v>
+        <v>180243.83</v>
       </c>
       <c r="H20" t="n">
-        <v>305263</v>
+        <v>519645</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1398,7 +1398,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1413,20 +1413,20 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>VnqKnEybGaw6G5ZAdjvPDri5RzDLPXznqxBunG13GJE</t>
+          <t>3vgopg7xm3EWkXfxmWPUpcf7g939hecfqg18sLuXDzVt</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.0001277</v>
+        <v>0.003843</v>
       </c>
       <c r="F21" t="n">
-        <v>11719.55</v>
+        <v>12245.11</v>
       </c>
       <c r="G21" t="n">
-        <v>56183.12</v>
+        <v>556084.9300000001</v>
       </c>
       <c r="H21" t="n">
-        <v>127726</v>
+        <v>3843154</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1445,7 +1445,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1460,20 +1460,20 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3vgopg7xm3EWkXfxmWPUpcf7g939hecfqg18sLuXDzVt</t>
+          <t>HD3JBABeFkdZwUgKwhwJYqjLNrPWXEaDVfH4uMqRpump</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.00385</v>
+        <v>0.0001759</v>
       </c>
       <c r="F22" t="n">
-        <v>10509.39</v>
+        <v>10514.78</v>
       </c>
       <c r="G22" t="n">
-        <v>553995.47</v>
+        <v>91162.82000000001</v>
       </c>
       <c r="H22" t="n">
-        <v>3850348</v>
+        <v>175918</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1492,7 +1492,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -1507,20 +1507,20 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>HD3JBABeFkdZwUgKwhwJYqjLNrPWXEaDVfH4uMqRpump</t>
+          <t>GuLvigFjAm1yyReTk6EeboHNnLj1tCi62pzWLorxbonk</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0.0001798</v>
+        <v>4.228e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>7314.19</v>
+        <v>8639.709999999999</v>
       </c>
       <c r="G23" t="n">
-        <v>91774.27</v>
+        <v>27091.54</v>
       </c>
       <c r="H23" t="n">
-        <v>179832</v>
+        <v>42287</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1539,7 +1539,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -1554,20 +1554,20 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>8erRtd8mLgNcNoWy2bhMdTgZyXaRR6u7t2hyXRc1pump</t>
+          <t>Et2bFLuPCW77hGW2g7UdrboPVuxatFZt4BaCzhCqpump</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>1.203e-05</v>
+        <v>0.0002897</v>
       </c>
       <c r="F24" t="n">
-        <v>5844.94</v>
+        <v>7982.32</v>
       </c>
       <c r="G24" t="n">
-        <v>14176.25</v>
+        <v>65917.89999999999</v>
       </c>
       <c r="H24" t="n">
-        <v>11996</v>
+        <v>289798</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1586,7 +1586,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -1601,20 +1601,20 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Et2bFLuPCW77hGW2g7UdrboPVuxatFZt4BaCzhCqpump</t>
+          <t>AMKKkovbUqr5cxmsg22KxTgaRXq6z4f8umrze4JKpump</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.0002742</v>
+        <v>0.0005211</v>
       </c>
       <c r="F25" t="n">
-        <v>5555.54</v>
+        <v>5451.82</v>
       </c>
       <c r="G25" t="n">
-        <v>63945.79</v>
+        <v>88426.64999999999</v>
       </c>
       <c r="H25" t="n">
-        <v>274285</v>
+        <v>372177</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -1633,7 +1633,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1648,20 +1648,20 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>AMKKkovbUqr5cxmsg22KxTgaRXq6z4f8umrze4JKpump</t>
+          <t>VnqKnEybGaw6G5ZAdjvPDri5RzDLPXznqxBunG13GJE</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.0004921</v>
+        <v>0.0001331</v>
       </c>
       <c r="F26" t="n">
-        <v>4374.56</v>
+        <v>4520.26</v>
       </c>
       <c r="G26" t="n">
-        <v>85525.23</v>
+        <v>57725.3</v>
       </c>
       <c r="H26" t="n">
-        <v>351482</v>
+        <v>133037</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1680,7 +1680,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1695,20 +1695,20 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>GuLvigFjAm1yyReTk6EeboHNnLj1tCi62pzWLorxbonk</t>
+          <t>8erRtd8mLgNcNoWy2bhMdTgZyXaRR6u7t2hyXRc1pump</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>4.497e-05</v>
+        <v>1.164e-05</v>
       </c>
       <c r="F27" t="n">
-        <v>4154.15</v>
+        <v>3411.79</v>
       </c>
       <c r="G27" t="n">
-        <v>27831.28</v>
+        <v>14087.13</v>
       </c>
       <c r="H27" t="n">
-        <v>44978</v>
+        <v>11610</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1727,7 +1727,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1742,20 +1742,20 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>GS3pHMUtYSu5PPuDFey74frkiRQhPdvx8jEeN6Qzbonk</t>
+          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>1.183e-05</v>
+        <v>3.652e-05</v>
       </c>
       <c r="F28" t="n">
-        <v>3872.16</v>
+        <v>3069.02</v>
       </c>
       <c r="G28" t="n">
-        <v>11923.77</v>
+        <v>25783.4</v>
       </c>
       <c r="H28" t="n">
-        <v>11840</v>
+        <v>36523</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1774,35 +1774,35 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>nan</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
+          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>3.879e-05</v>
+        <v>1534.13</v>
       </c>
       <c r="F29" t="n">
-        <v>3709.02</v>
+        <v>3052.89</v>
       </c>
       <c r="G29" t="n">
-        <v>26391.69</v>
+        <v>20927.71</v>
       </c>
       <c r="H29" t="n">
-        <v>38789</v>
+        <v>24776305</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1821,35 +1821,35 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>nan</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
+          <t>LGiKAMtb4BuPdhpThjEbNWbDddqdM5FnxMMHqtzpump</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>1529.97</v>
+        <v>1.151e-05</v>
       </c>
       <c r="F30" t="n">
-        <v>2990.61</v>
+        <v>2858.96</v>
       </c>
       <c r="G30" t="n">
-        <v>20811.94</v>
+        <v>14760.12</v>
       </c>
       <c r="H30" t="n">
-        <v>24709085</v>
+        <v>11513</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -1868,7 +1868,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1883,20 +1883,20 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>LGiKAMtb4BuPdhpThjEbNWbDddqdM5FnxMMHqtzpump</t>
+          <t>9h5y3WCqfeNt2fiAP7iM2ZRp9apFb58ipvTzcWi9pump</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.281e-05</v>
+        <v>2.743e-05</v>
       </c>
       <c r="F31" t="n">
-        <v>1938.11</v>
+        <v>2720.45</v>
       </c>
       <c r="G31" t="n">
-        <v>15475.67</v>
+        <v>24490.89</v>
       </c>
       <c r="H31" t="n">
-        <v>12813</v>
+        <v>27434</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1915,7 +1915,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1930,20 +1930,20 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14GMPMf3cRANLfJ9QYU19F5XogVGPjCB7f3NLACrpump</t>
+          <t>HW2B2wvyEir3iqvYbYqbHWyR7rA6DqCR3WQSy4USpump</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>2.658e-05</v>
+        <v>3.348e-05</v>
       </c>
       <c r="F32" t="n">
-        <v>1529.3</v>
+        <v>2551.2</v>
       </c>
       <c r="G32" t="n">
-        <v>20795.82</v>
+        <v>22322.38</v>
       </c>
       <c r="H32" t="n">
-        <v>26317</v>
+        <v>33481</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
@@ -1962,7 +1962,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1977,20 +1977,20 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>9zFU5vR7YNBzZU8HwJLUKjoDEonpgvHUdLbMgBa7pump</t>
+          <t>GS3pHMUtYSu5PPuDFey74frkiRQhPdvx8jEeN6Qzbonk</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>1.599e-05</v>
+        <v>1.189e-05</v>
       </c>
       <c r="F33" t="n">
-        <v>1516.53</v>
+        <v>2302.48</v>
       </c>
       <c r="G33" t="n">
-        <v>16044.6</v>
+        <v>11951.64</v>
       </c>
       <c r="H33" t="n">
-        <v>15906</v>
+        <v>11894</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -2009,7 +2009,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2024,20 +2024,20 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>4CBToKTRKfBsv8RMfzMr6VfKQ8PLRYeG6RFGZmq4pump</t>
+          <t>14GMPMf3cRANLfJ9QYU19F5XogVGPjCB7f3NLACrpump</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1.364e-05</v>
+        <v>2.641e-05</v>
       </c>
       <c r="F34" t="n">
-        <v>1426.58</v>
+        <v>2104.89</v>
       </c>
       <c r="G34" t="n">
-        <v>16572.63</v>
+        <v>20890.58</v>
       </c>
       <c r="H34" t="n">
-        <v>13405</v>
+        <v>26143</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -2056,7 +2056,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2071,20 +2071,20 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>9h5y3WCqfeNt2fiAP7iM2ZRp9apFb58ipvTzcWi9pump</t>
+          <t>qG9NJP4pgFxWWfpFWV7GcYkTKyafDGsnUGCDZLRpump</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2.702e-05</v>
+        <v>4.896e-06</v>
       </c>
       <c r="F35" t="n">
-        <v>1187.47</v>
+        <v>1801.61</v>
       </c>
       <c r="G35" t="n">
-        <v>24197.39</v>
+        <v>8547.309999999999</v>
       </c>
       <c r="H35" t="n">
-        <v>27022</v>
+        <v>4895</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -2103,7 +2103,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -2118,20 +2118,20 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
+          <t>9zFU5vR7YNBzZU8HwJLUKjoDEonpgvHUdLbMgBa7pump</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>1.423e-07</v>
+        <v>1.862e-05</v>
       </c>
       <c r="F36" t="n">
-        <v>1165.6</v>
+        <v>1790.89</v>
       </c>
       <c r="G36" t="n">
-        <v>10940.63</v>
+        <v>17391.74</v>
       </c>
       <c r="H36" t="n">
-        <v>9824</v>
+        <v>18528</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -2150,7 +2150,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -2165,20 +2165,20 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>HW2B2wvyEir3iqvYbYqbHWyR7rA6DqCR3WQSy4USpump</t>
+          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2.829e-05</v>
+        <v>1.229e-07</v>
       </c>
       <c r="F37" t="n">
-        <v>1152.29</v>
+        <v>1575.01</v>
       </c>
       <c r="G37" t="n">
-        <v>20418.95</v>
+        <v>10193.12</v>
       </c>
       <c r="H37" t="n">
-        <v>28292</v>
+        <v>8487</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2197,7 +2197,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -2212,20 +2212,20 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>DKffyw1oEVWR3ik7q7tb2shhmZ3jbTkRzT6R5banCxai</t>
+          <t>8wbfBYthc9fC4GsHgCtznZP1PAoXaZ8tnUGBtGMgpump</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>1.18</v>
+        <v>8.355999999999999e-06</v>
       </c>
       <c r="F38" t="n">
-        <v>888.89</v>
+        <v>1298.42</v>
       </c>
       <c r="G38" t="n">
-        <v>2680592.35</v>
+        <v>12263</v>
       </c>
       <c r="H38" t="n">
-        <v>24926825</v>
+        <v>8353</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -2244,7 +2244,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2259,20 +2259,20 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>8wbfBYthc9fC4GsHgCtznZP1PAoXaZ8tnUGBtGMgpump</t>
+          <t>DKffyw1oEVWR3ik7q7tb2shhmZ3jbTkRzT6R5banCxai</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>8.073e-06</v>
+        <v>1.21</v>
       </c>
       <c r="F39" t="n">
-        <v>872.05</v>
+        <v>1035.12</v>
       </c>
       <c r="G39" t="n">
-        <v>11981.52</v>
+        <v>2731801.19</v>
       </c>
       <c r="H39" t="n">
-        <v>8071</v>
+        <v>25451264</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2291,7 +2291,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -2306,20 +2306,20 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>EVGox5PPxnFqTsMXMoUBSCUhszqK6UUYf9W7pkwfpump</t>
+          <t>4CBToKTRKfBsv8RMfzMr6VfKQ8PLRYeG6RFGZmq4pump</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>3.063e-05</v>
+        <v>1.378e-05</v>
       </c>
       <c r="F40" t="n">
-        <v>657.45</v>
+        <v>1029.84</v>
       </c>
       <c r="G40" t="n">
-        <v>21986.51</v>
+        <v>16734.48</v>
       </c>
       <c r="H40" t="n">
-        <v>30630</v>
+        <v>13541</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -2338,7 +2338,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -2353,20 +2353,20 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>qG9NJP4pgFxWWfpFWV7GcYkTKyafDGsnUGCDZLRpump</t>
+          <t>EVGox5PPxnFqTsMXMoUBSCUhszqK6UUYf9W7pkwfpump</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>4.61e-06</v>
+        <v>3.081e-05</v>
       </c>
       <c r="F41" t="n">
-        <v>542.4400000000001</v>
+        <v>556.33</v>
       </c>
       <c r="G41" t="n">
-        <v>8256.75</v>
+        <v>22064.03</v>
       </c>
       <c r="H41" t="n">
-        <v>4610</v>
+        <v>30818</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -2385,7 +2385,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -2404,16 +2404,16 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>1.883e-05</v>
+        <v>1.845e-05</v>
       </c>
       <c r="F42" t="n">
-        <v>468.89</v>
+        <v>513.33</v>
       </c>
       <c r="G42" t="n">
-        <v>25197.89</v>
+        <v>25059.06</v>
       </c>
       <c r="H42" t="n">
-        <v>18830</v>
+        <v>18447</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
@@ -2432,7 +2432,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -2451,16 +2451,16 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>1.009e-05</v>
+        <v>9.305e-06</v>
       </c>
       <c r="F43" t="n">
-        <v>391.69</v>
+        <v>417.55</v>
       </c>
       <c r="G43" t="n">
-        <v>12971.75</v>
+        <v>12510.17</v>
       </c>
       <c r="H43" t="n">
-        <v>10095</v>
+        <v>9305</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -2479,7 +2479,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -2498,16 +2498,16 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>5.696e-06</v>
+        <v>5.189e-06</v>
       </c>
       <c r="F44" t="n">
-        <v>361</v>
+        <v>234.89</v>
       </c>
       <c r="G44" t="n">
-        <v>4860.64</v>
+        <v>4669.96</v>
       </c>
       <c r="H44" t="n">
-        <v>5697</v>
+        <v>5190</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -2526,7 +2526,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -2545,16 +2545,16 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>7.547e-06</v>
+        <v>7.669999999999999e-06</v>
       </c>
       <c r="F45" t="n">
-        <v>142.24</v>
+        <v>165.21</v>
       </c>
       <c r="G45" t="n">
-        <v>10674.86</v>
+        <v>10821.66</v>
       </c>
       <c r="H45" t="n">
-        <v>7543</v>
+        <v>7666</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -2573,7 +2573,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2588,20 +2588,20 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>8D7n3WYZxUkmhUPveQU4XZdqLfDe4XLEEpPToAk4pump</t>
+          <t>CmLrhRd762bfytq6f3ZV5iuivN1Q8oyPw4evyW4Mbonk</t>
         </is>
       </c>
       <c r="E46" t="n">
-        <v>5.984e-06</v>
+        <v>6.143e-06</v>
       </c>
       <c r="F46" t="n">
-        <v>103.97</v>
+        <v>94.36</v>
       </c>
       <c r="G46" t="n">
-        <v>0</v>
+        <v>9871.129999999999</v>
       </c>
       <c r="H46" t="n">
-        <v>5984.88</v>
+        <v>6143</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -2620,7 +2620,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2635,20 +2635,20 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>CmLrhRd762bfytq6f3ZV5iuivN1Q8oyPw4evyW4Mbonk</t>
+          <t>CAamcXXVWM8b8DcpcT2rpEwwfNfBD2MXjHjCwRDBpump</t>
         </is>
       </c>
       <c r="E47" t="n">
-        <v>6.085e-06</v>
+        <v>9.095e-06</v>
       </c>
       <c r="F47" t="n">
-        <v>87.95999999999999</v>
+        <v>48.16</v>
       </c>
       <c r="G47" t="n">
-        <v>9748.07</v>
+        <v>11995.44</v>
       </c>
       <c r="H47" t="n">
-        <v>6085</v>
+        <v>9093</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
@@ -2667,7 +2667,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -2682,20 +2682,20 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>EzcwA7anSrdoH1TMKjbBTd91GD7KwMco9kFZh1AApump</t>
+          <t>4bLnK5YuJaqkVX4uWtJ1Qtx3XoZ8eHH37STXSwujpump</t>
         </is>
       </c>
       <c r="E48" t="n">
-        <v>5.64e-06</v>
+        <v>9.004999999999999e-06</v>
       </c>
       <c r="F48" t="n">
-        <v>29.82</v>
+        <v>48.09</v>
       </c>
       <c r="G48" t="n">
-        <v>8990.33</v>
+        <v>13248.38</v>
       </c>
       <c r="H48" t="n">
-        <v>5638</v>
+        <v>8916</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -2714,7 +2714,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -2729,20 +2729,20 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>HpQUbEAcHrhwSJyYfXLNZvJz9SBksRJJStn86gFdbonk</t>
+          <t>EzcwA7anSrdoH1TMKjbBTd91GD7KwMco9kFZh1AApump</t>
         </is>
       </c>
       <c r="E49" t="n">
-        <v>4.74e-06</v>
+        <v>5.782e-06</v>
       </c>
       <c r="F49" t="n">
-        <v>25.13</v>
+        <v>29.95</v>
       </c>
       <c r="G49" t="n">
-        <v>7226.09</v>
+        <v>9246.780000000001</v>
       </c>
       <c r="H49" t="n">
-        <v>4740</v>
+        <v>5780</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -2761,7 +2761,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2780,16 +2780,16 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0.01246</v>
+        <v>0.01293</v>
       </c>
       <c r="F50" t="n">
-        <v>16.25</v>
+        <v>25.78</v>
       </c>
       <c r="G50" t="n">
-        <v>7386.82</v>
+        <v>7645.7</v>
       </c>
       <c r="H50" t="n">
-        <v>12462</v>
+        <v>12932</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -2808,7 +2808,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2025-09-28</t>
+          <t>2025-09-29</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -2823,20 +2823,20 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>iD9FqgeKmp58a4pTvh45MtKkHkudKNptFRdR8m6pump</t>
+          <t>8D7n3WYZxUkmhUPveQU4XZdqLfDe4XLEEpPToAk4pump</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>4.777e-06</v>
+        <v>5.984e-06</v>
       </c>
       <c r="F51" t="n">
-        <v>16.09</v>
+        <v>24.38</v>
       </c>
       <c r="G51" t="n">
-        <v>8261.280000000001</v>
+        <v>0</v>
       </c>
       <c r="H51" t="n">
-        <v>4777</v>
+        <v>5984.88</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
chore: update reports (2025-10-01)
</commit_message>
<xml_diff>
--- a/sol_master_LIVE.xlsx
+++ b/sol_master_LIVE.xlsx
@@ -532,13 +532,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>217.3</v>
+        <v>217.67</v>
       </c>
       <c r="F2" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="G2" t="n">
-        <v>55068304.14</v>
+        <v>55374839.99</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -579,16 +579,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.0001467</v>
+        <v>0.0001641</v>
       </c>
       <c r="F3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="G3" t="n">
-        <v>79895.31</v>
+        <v>83232.7</v>
       </c>
       <c r="H3" t="n">
-        <v>146749</v>
+        <v>164163</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -626,16 +626,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.001647</v>
+        <v>0.0016</v>
       </c>
       <c r="F4" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="G4" t="n">
-        <v>224085.03</v>
+        <v>221116.95</v>
       </c>
       <c r="H4" t="n">
-        <v>1280147</v>
+        <v>1244218</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -673,16 +673,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.002688</v>
+        <v>0.00269</v>
       </c>
       <c r="F5" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="G5" t="n">
-        <v>500882.98</v>
+        <v>501076.47</v>
       </c>
       <c r="H5" t="n">
-        <v>2686803</v>
+        <v>2688607</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -720,16 +720,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.0004236</v>
+        <v>0.0004245</v>
       </c>
       <c r="F6" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="G6" t="n">
-        <v>124024.45</v>
+        <v>124317.64</v>
       </c>
       <c r="H6" t="n">
-        <v>423594</v>
+        <v>424479</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -767,16 +767,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.0001839</v>
+        <v>0.0001816</v>
       </c>
       <c r="F7" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="G7" t="n">
-        <v>53759.6</v>
+        <v>53430.12</v>
       </c>
       <c r="H7" t="n">
-        <v>183981</v>
+        <v>181694</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -814,16 +814,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.0008705</v>
+        <v>0.0008823</v>
       </c>
       <c r="F8" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="G8" t="n">
-        <v>199804.55</v>
+        <v>201193.35</v>
       </c>
       <c r="H8" t="n">
-        <v>870510</v>
+        <v>882390</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -861,16 +861,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.001813</v>
+        <v>0.001829</v>
       </c>
       <c r="F9" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="G9" t="n">
-        <v>189799.17</v>
+        <v>190853.78</v>
       </c>
       <c r="H9" t="n">
-        <v>1813152</v>
+        <v>1829689</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -911,7 +911,7 @@
         <v>0.0002214</v>
       </c>
       <c r="F10" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="G10" t="n">
         <v>58993.73</v>
@@ -955,16 +955,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.01617</v>
+        <v>0.01623</v>
       </c>
       <c r="F11" t="n">
-        <v>83707.00999999999</v>
+        <v>82202</v>
       </c>
       <c r="G11" t="n">
-        <v>2105164.95</v>
+        <v>2110607.3</v>
       </c>
       <c r="H11" t="n">
-        <v>80878379</v>
+        <v>81173576</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
         <v>0.00111</v>
       </c>
       <c r="F12" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="G12" t="n">
         <v>166013.41</v>
@@ -1052,7 +1052,7 @@
         <v>0.0006933</v>
       </c>
       <c r="F13" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="G13" t="n">
         <v>104294.04</v>
@@ -1096,16 +1096,16 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.0004602</v>
+        <v>0.0004622</v>
       </c>
       <c r="F14" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="G14" t="n">
-        <v>138294.92</v>
+        <v>138661.32</v>
       </c>
       <c r="H14" t="n">
-        <v>460190</v>
+        <v>462204</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1143,16 +1143,16 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.0002183</v>
+        <v>0.0002218</v>
       </c>
       <c r="F15" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="G15" t="n">
-        <v>74040.59</v>
+        <v>74592.92999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>217631</v>
+        <v>221086</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -1190,16 +1190,16 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.0005199</v>
+        <v>0.0005284000000000001</v>
       </c>
       <c r="F16" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="G16" t="n">
-        <v>148065.02</v>
+        <v>149501</v>
       </c>
       <c r="H16" t="n">
-        <v>519796</v>
+        <v>528322</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1240,7 +1240,7 @@
         <v>0.000112</v>
       </c>
       <c r="F17" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="G17" t="n">
         <v>56740.29</v>
@@ -1284,16 +1284,16 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.0003056</v>
+        <v>0.0003025</v>
       </c>
       <c r="F18" t="n">
-        <v>38198.12</v>
+        <v>39570.21</v>
       </c>
       <c r="G18" t="n">
-        <v>72990.33</v>
+        <v>72811.57000000001</v>
       </c>
       <c r="H18" t="n">
-        <v>305574</v>
+        <v>302512</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -1331,16 +1331,16 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.0004733</v>
+        <v>0.0004963</v>
       </c>
       <c r="F19" t="n">
-        <v>31601.34</v>
+        <v>35912.32</v>
       </c>
       <c r="G19" t="n">
-        <v>175629.27</v>
+        <v>180047.48</v>
       </c>
       <c r="H19" t="n">
-        <v>473325</v>
+        <v>496394</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -1378,16 +1378,16 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>6.745999999999999e-05</v>
+        <v>6.567999999999999e-05</v>
       </c>
       <c r="F20" t="n">
-        <v>18225.35</v>
+        <v>18606.34</v>
       </c>
       <c r="G20" t="n">
-        <v>39289.74</v>
+        <v>38871.85</v>
       </c>
       <c r="H20" t="n">
-        <v>67461</v>
+        <v>65683</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -1411,30 +1411,30 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>VIBECODER</t>
+          <t>walkusa</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Vibe Coding Meta</t>
+          <t>WALKING ACROSS AMERICA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.0001341</v>
+        <v>7.773e-05</v>
       </c>
       <c r="F21" t="n">
-        <v>17344.55</v>
+        <v>17207.7</v>
       </c>
       <c r="G21" t="n">
-        <v>53854.17</v>
+        <v>38711.88</v>
       </c>
       <c r="H21" t="n">
-        <v>130146</v>
+        <v>77734</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -1458,30 +1458,30 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>walkusa</t>
+          <t>VIBECODER</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>WALKING ACROSS AMERICA</t>
+          <t>Vibe Coding Meta</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
+          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7.773e-05</v>
+        <v>0.0001341</v>
       </c>
       <c r="F22" t="n">
-        <v>17207.7</v>
+        <v>17176.84</v>
       </c>
       <c r="G22" t="n">
-        <v>38711.88</v>
+        <v>53854.17</v>
       </c>
       <c r="H22" t="n">
-        <v>77734</v>
+        <v>130146</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -1522,7 +1522,7 @@
         <v>6.069e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="G23" t="n">
         <v>31664.06</v>
@@ -1616,7 +1616,7 @@
         <v>0.000151</v>
       </c>
       <c r="F25" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="G25" t="n">
         <v>86166.2</v>
@@ -1660,16 +1660,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.003955</v>
+        <v>0.003962</v>
       </c>
       <c r="F26" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="G26" t="n">
-        <v>574364.5</v>
+        <v>576259.42</v>
       </c>
       <c r="H26" t="n">
-        <v>3955131</v>
+        <v>3962041</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -1707,16 +1707,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2.031e-05</v>
+        <v>2.048e-05</v>
       </c>
       <c r="F27" t="n">
-        <v>6301.32</v>
+        <v>6314.15</v>
       </c>
       <c r="G27" t="n">
-        <v>9398.59</v>
+        <v>9452.41</v>
       </c>
       <c r="H27" t="n">
-        <v>20312</v>
+        <v>20483</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -1754,16 +1754,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.0001347</v>
+        <v>0.0001337</v>
       </c>
       <c r="F28" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="G28" t="n">
-        <v>59174.67</v>
+        <v>59068.31</v>
       </c>
       <c r="H28" t="n">
-        <v>134692</v>
+        <v>133707</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -1801,16 +1801,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2.046e-05</v>
+        <v>2.067e-05</v>
       </c>
       <c r="F29" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="G29" t="n">
-        <v>18773.74</v>
+        <v>18886.56</v>
       </c>
       <c r="H29" t="n">
-        <v>20262</v>
+        <v>20468</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -1851,7 +1851,7 @@
         <v>1.243e-05</v>
       </c>
       <c r="F30" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="G30" t="n">
         <v>12272.48</v>
@@ -1895,16 +1895,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.276e-05</v>
+        <v>1.299e-05</v>
       </c>
       <c r="F31" t="n">
-        <v>2590.53</v>
+        <v>2697.91</v>
       </c>
       <c r="G31" t="n">
-        <v>15027.69</v>
+        <v>15181.74</v>
       </c>
       <c r="H31" t="n">
-        <v>12730</v>
+        <v>12959</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -1945,7 +1945,7 @@
         <v>2.155e-05</v>
       </c>
       <c r="F32" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="G32" t="n">
         <v>19038.67</v>
@@ -2022,30 +2022,30 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>IDIOT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>IDIOT</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
+          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1649.46</v>
+        <v>2.909e-05</v>
       </c>
       <c r="F34" t="n">
-        <v>2288.31</v>
+        <v>2431.43</v>
       </c>
       <c r="G34" t="n">
-        <v>14828.26</v>
+        <v>23502.49</v>
       </c>
       <c r="H34" t="n">
-        <v>26638843</v>
+        <v>29094</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -2069,30 +2069,30 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RWA</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Real World Asses</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
+          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>9.666000000000001e-08</v>
+        <v>1646.86</v>
       </c>
       <c r="F35" t="n">
-        <v>2243.13</v>
+        <v>2306.05</v>
       </c>
       <c r="G35" t="n">
-        <v>9081.24</v>
+        <v>14826.8</v>
       </c>
       <c r="H35" t="n">
-        <v>6670</v>
+        <v>26596804</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -2116,30 +2116,30 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>IDIOT</t>
+          <t>RWA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>IDIOT</t>
+          <t>Real World Asses</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
+          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2.942e-05</v>
+        <v>9.504999999999999e-08</v>
       </c>
       <c r="F36" t="n">
-        <v>1830.81</v>
+        <v>2279.84</v>
       </c>
       <c r="G36" t="n">
-        <v>23157.24</v>
+        <v>9007.809999999999</v>
       </c>
       <c r="H36" t="n">
-        <v>29426</v>
+        <v>6559</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -2177,16 +2177,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2.993e-05</v>
+        <v>2.96e-05</v>
       </c>
       <c r="F37" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="G37" t="n">
-        <v>21480.66</v>
+        <v>21416.84</v>
       </c>
       <c r="H37" t="n">
-        <v>29934</v>
+        <v>29604</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -2271,16 +2271,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1.04e-05</v>
+        <v>1.036e-05</v>
       </c>
       <c r="F39" t="n">
-        <v>1355.84</v>
+        <v>1376.56</v>
       </c>
       <c r="G39" t="n">
-        <v>13484.99</v>
+        <v>13472.6</v>
       </c>
       <c r="H39" t="n">
-        <v>10409</v>
+        <v>10363</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -2318,16 +2318,16 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2.259e-05</v>
+        <v>2.326e-05</v>
       </c>
       <c r="F40" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="G40" t="n">
-        <v>22300.62</v>
+        <v>23013.57</v>
       </c>
       <c r="H40" t="n">
-        <v>22594</v>
+        <v>23265</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -2821,30 +2821,30 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FLY</t>
+          <t>grandma</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Nexa</t>
+          <t>101 Year Old Pumpfun Livestreamr</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>9NcUwy9JVekfsY4UA62ZaTprn4TDnJZwp5B6vMAAtkzt</t>
+          <t>4CBToKTRKfBsv8RMfzMr6VfKQ8PLRYeG6RFGZmq4pump</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.01399</v>
+        <v>1.323e-05</v>
       </c>
       <c r="F51" t="n">
-        <v>45.53</v>
+        <v>54.86</v>
       </c>
       <c r="G51" t="n">
-        <v>8095.6</v>
+        <v>16735.19</v>
       </c>
       <c r="H51" t="n">
-        <v>13996</v>
+        <v>13005</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -7514,22 +7514,22 @@
         <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>217.3</v>
+        <v>217.67</v>
       </c>
       <c r="H2" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="I2" t="n">
-        <v>55068304.14</v>
+        <v>55374839.99</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="L2" t="n">
-        <v>55068304.14</v>
+        <v>55374839.99</v>
       </c>
       <c r="M2" t="n">
         <v>1</v>
@@ -7567,22 +7567,22 @@
         <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0001467</v>
+        <v>0.0001641</v>
       </c>
       <c r="H3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="I3" t="n">
-        <v>79895.31</v>
+        <v>83232.7</v>
       </c>
       <c r="J3" t="n">
-        <v>146749</v>
+        <v>164163</v>
       </c>
       <c r="K3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="L3" t="n">
-        <v>79895.31</v>
+        <v>83232.7</v>
       </c>
       <c r="M3" t="n">
         <v>1</v>
@@ -7620,22 +7620,22 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.001647</v>
+        <v>0.0016</v>
       </c>
       <c r="H4" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="I4" t="n">
-        <v>224085.03</v>
+        <v>221116.95</v>
       </c>
       <c r="J4" t="n">
-        <v>1280147</v>
+        <v>1244218</v>
       </c>
       <c r="K4" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="L4" t="n">
-        <v>224085.03</v>
+        <v>221116.95</v>
       </c>
       <c r="M4" t="n">
         <v>1</v>
@@ -7673,22 +7673,22 @@
         <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>0.002688</v>
+        <v>0.00269</v>
       </c>
       <c r="H5" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="I5" t="n">
-        <v>500882.98</v>
+        <v>501076.47</v>
       </c>
       <c r="J5" t="n">
-        <v>2686803</v>
+        <v>2688607</v>
       </c>
       <c r="K5" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="L5" t="n">
-        <v>500882.98</v>
+        <v>501076.47</v>
       </c>
       <c r="M5" t="n">
         <v>1</v>
@@ -7726,22 +7726,22 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0004236</v>
+        <v>0.0004245</v>
       </c>
       <c r="H6" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="I6" t="n">
-        <v>124024.45</v>
+        <v>124317.64</v>
       </c>
       <c r="J6" t="n">
-        <v>423594</v>
+        <v>424479</v>
       </c>
       <c r="K6" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="L6" t="n">
-        <v>124024.45</v>
+        <v>124317.64</v>
       </c>
       <c r="M6" t="n">
         <v>1</v>
@@ -7779,22 +7779,22 @@
         <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0001839</v>
+        <v>0.0001816</v>
       </c>
       <c r="H7" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="I7" t="n">
-        <v>53759.6</v>
+        <v>53430.12</v>
       </c>
       <c r="J7" t="n">
-        <v>183981</v>
+        <v>181694</v>
       </c>
       <c r="K7" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="L7" t="n">
-        <v>53759.6</v>
+        <v>53430.12</v>
       </c>
       <c r="M7" t="n">
         <v>1</v>
@@ -7832,22 +7832,22 @@
         <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0008705</v>
+        <v>0.0008823</v>
       </c>
       <c r="H8" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="I8" t="n">
-        <v>199804.55</v>
+        <v>201193.35</v>
       </c>
       <c r="J8" t="n">
-        <v>870510</v>
+        <v>882390</v>
       </c>
       <c r="K8" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="L8" t="n">
-        <v>199804.55</v>
+        <v>201193.35</v>
       </c>
       <c r="M8" t="n">
         <v>1</v>
@@ -7885,22 +7885,22 @@
         <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>0.001813</v>
+        <v>0.001829</v>
       </c>
       <c r="H9" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="I9" t="n">
-        <v>189799.17</v>
+        <v>190853.78</v>
       </c>
       <c r="J9" t="n">
-        <v>1813152</v>
+        <v>1829689</v>
       </c>
       <c r="K9" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="L9" t="n">
-        <v>189799.17</v>
+        <v>190853.78</v>
       </c>
       <c r="M9" t="n">
         <v>1</v>
@@ -7941,7 +7941,7 @@
         <v>0.0002214</v>
       </c>
       <c r="H10" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="I10" t="n">
         <v>58993.73</v>
@@ -7950,7 +7950,7 @@
         <v>221404</v>
       </c>
       <c r="K10" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="L10" t="n">
         <v>58993.73</v>
@@ -7991,22 +7991,22 @@
         <v>1</v>
       </c>
       <c r="G11" t="n">
-        <v>0.01617</v>
+        <v>0.01623</v>
       </c>
       <c r="H11" t="n">
-        <v>83707.00999999999</v>
+        <v>82202</v>
       </c>
       <c r="I11" t="n">
-        <v>2105164.95</v>
+        <v>2110607.3</v>
       </c>
       <c r="J11" t="n">
-        <v>80878379</v>
+        <v>81173576</v>
       </c>
       <c r="K11" t="n">
-        <v>83707.00999999999</v>
+        <v>82202</v>
       </c>
       <c r="L11" t="n">
-        <v>2105164.95</v>
+        <v>2110607.3</v>
       </c>
       <c r="M11" t="n">
         <v>1</v>
@@ -8047,7 +8047,7 @@
         <v>0.00111</v>
       </c>
       <c r="H12" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="I12" t="n">
         <v>166013.41</v>
@@ -8056,7 +8056,7 @@
         <v>1109964</v>
       </c>
       <c r="K12" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="L12" t="n">
         <v>166013.41</v>
@@ -8100,7 +8100,7 @@
         <v>0.0006933</v>
       </c>
       <c r="H13" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="I13" t="n">
         <v>104294.04</v>
@@ -8109,7 +8109,7 @@
         <v>495120</v>
       </c>
       <c r="K13" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="L13" t="n">
         <v>104294.04</v>
@@ -8150,22 +8150,22 @@
         <v>1</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0004602</v>
+        <v>0.0004622</v>
       </c>
       <c r="H14" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="I14" t="n">
-        <v>138294.92</v>
+        <v>138661.32</v>
       </c>
       <c r="J14" t="n">
-        <v>460190</v>
+        <v>462204</v>
       </c>
       <c r="K14" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="L14" t="n">
-        <v>138294.92</v>
+        <v>138661.32</v>
       </c>
       <c r="M14" t="n">
         <v>1</v>
@@ -8203,22 +8203,22 @@
         <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0002183</v>
+        <v>0.0002218</v>
       </c>
       <c r="H15" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="I15" t="n">
-        <v>74040.59</v>
+        <v>74592.92999999999</v>
       </c>
       <c r="J15" t="n">
-        <v>217631</v>
+        <v>221086</v>
       </c>
       <c r="K15" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="L15" t="n">
-        <v>74040.59</v>
+        <v>74592.92999999999</v>
       </c>
       <c r="M15" t="n">
         <v>1</v>
@@ -8256,22 +8256,22 @@
         <v>1</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0005199</v>
+        <v>0.0005284000000000001</v>
       </c>
       <c r="H16" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="I16" t="n">
-        <v>148065.02</v>
+        <v>149501</v>
       </c>
       <c r="J16" t="n">
-        <v>519796</v>
+        <v>528322</v>
       </c>
       <c r="K16" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="L16" t="n">
-        <v>148065.02</v>
+        <v>149501</v>
       </c>
       <c r="M16" t="n">
         <v>1</v>
@@ -8312,7 +8312,7 @@
         <v>0.000112</v>
       </c>
       <c r="H17" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="I17" t="n">
         <v>56740.29</v>
@@ -8321,7 +8321,7 @@
         <v>111863</v>
       </c>
       <c r="K17" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="L17" t="n">
         <v>56740.29</v>
@@ -8362,22 +8362,22 @@
         <v>1</v>
       </c>
       <c r="G18" t="n">
-        <v>0.0003056</v>
+        <v>0.0003025</v>
       </c>
       <c r="H18" t="n">
-        <v>38198.12</v>
+        <v>39570.21</v>
       </c>
       <c r="I18" t="n">
-        <v>72990.33</v>
+        <v>72811.57000000001</v>
       </c>
       <c r="J18" t="n">
-        <v>305574</v>
+        <v>302512</v>
       </c>
       <c r="K18" t="n">
-        <v>38198.12</v>
+        <v>39570.21</v>
       </c>
       <c r="L18" t="n">
-        <v>72990.33</v>
+        <v>72811.57000000001</v>
       </c>
       <c r="M18" t="n">
         <v>1</v>
@@ -8415,22 +8415,22 @@
         <v>1</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0004733</v>
+        <v>0.0004963</v>
       </c>
       <c r="H19" t="n">
-        <v>31601.34</v>
+        <v>35912.32</v>
       </c>
       <c r="I19" t="n">
-        <v>175629.27</v>
+        <v>180047.48</v>
       </c>
       <c r="J19" t="n">
-        <v>473325</v>
+        <v>496394</v>
       </c>
       <c r="K19" t="n">
-        <v>31601.34</v>
+        <v>35912.32</v>
       </c>
       <c r="L19" t="n">
-        <v>175629.27</v>
+        <v>180047.48</v>
       </c>
       <c r="M19" t="n">
         <v>1</v>
@@ -8468,22 +8468,22 @@
         <v>1</v>
       </c>
       <c r="G20" t="n">
-        <v>6.745999999999999e-05</v>
+        <v>6.567999999999999e-05</v>
       </c>
       <c r="H20" t="n">
-        <v>18225.35</v>
+        <v>18606.34</v>
       </c>
       <c r="I20" t="n">
-        <v>39289.74</v>
+        <v>38871.85</v>
       </c>
       <c r="J20" t="n">
-        <v>67461</v>
+        <v>65683</v>
       </c>
       <c r="K20" t="n">
-        <v>18225.35</v>
+        <v>18606.34</v>
       </c>
       <c r="L20" t="n">
-        <v>39289.74</v>
+        <v>38871.85</v>
       </c>
       <c r="M20" t="n">
         <v>1</v>
@@ -8498,17 +8498,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>VIBECODER</t>
+          <t>walkusa</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Vibe Coding Meta</t>
+          <t>WALKING ACROSS AMERICA</t>
         </is>
       </c>
       <c r="D21" s="2" t="n">
@@ -8521,22 +8521,22 @@
         <v>1</v>
       </c>
       <c r="G21" t="n">
-        <v>0.0001341</v>
+        <v>7.773e-05</v>
       </c>
       <c r="H21" t="n">
-        <v>17344.55</v>
+        <v>17207.7</v>
       </c>
       <c r="I21" t="n">
-        <v>53854.17</v>
+        <v>38711.88</v>
       </c>
       <c r="J21" t="n">
-        <v>130146</v>
+        <v>77734</v>
       </c>
       <c r="K21" t="n">
-        <v>17344.55</v>
+        <v>17207.7</v>
       </c>
       <c r="L21" t="n">
-        <v>53854.17</v>
+        <v>38711.88</v>
       </c>
       <c r="M21" t="n">
         <v>1</v>
@@ -8551,17 +8551,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
+          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>walkusa</t>
+          <t>VIBECODER</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>WALKING ACROSS AMERICA</t>
+          <t>Vibe Coding Meta</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
@@ -8574,22 +8574,22 @@
         <v>1</v>
       </c>
       <c r="G22" t="n">
-        <v>7.773e-05</v>
+        <v>0.0001341</v>
       </c>
       <c r="H22" t="n">
-        <v>17207.7</v>
+        <v>17176.84</v>
       </c>
       <c r="I22" t="n">
-        <v>38711.88</v>
+        <v>53854.17</v>
       </c>
       <c r="J22" t="n">
-        <v>77734</v>
+        <v>130146</v>
       </c>
       <c r="K22" t="n">
-        <v>17207.7</v>
+        <v>17176.84</v>
       </c>
       <c r="L22" t="n">
-        <v>38711.88</v>
+        <v>53854.17</v>
       </c>
       <c r="M22" t="n">
         <v>1</v>
@@ -8630,7 +8630,7 @@
         <v>6.069e-05</v>
       </c>
       <c r="H23" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="I23" t="n">
         <v>31664.06</v>
@@ -8639,7 +8639,7 @@
         <v>60689</v>
       </c>
       <c r="K23" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="L23" t="n">
         <v>31664.06</v>
@@ -8736,7 +8736,7 @@
         <v>0.000151</v>
       </c>
       <c r="H25" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="I25" t="n">
         <v>86166.2</v>
@@ -8745,7 +8745,7 @@
         <v>151047</v>
       </c>
       <c r="K25" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="L25" t="n">
         <v>86166.2</v>
@@ -8786,22 +8786,22 @@
         <v>1</v>
       </c>
       <c r="G26" t="n">
-        <v>0.003955</v>
+        <v>0.003962</v>
       </c>
       <c r="H26" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="I26" t="n">
-        <v>574364.5</v>
+        <v>576259.42</v>
       </c>
       <c r="J26" t="n">
-        <v>3955131</v>
+        <v>3962041</v>
       </c>
       <c r="K26" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="L26" t="n">
-        <v>574364.5</v>
+        <v>576259.42</v>
       </c>
       <c r="M26" t="n">
         <v>1</v>
@@ -8839,22 +8839,22 @@
         <v>1</v>
       </c>
       <c r="G27" t="n">
-        <v>2.031e-05</v>
+        <v>2.048e-05</v>
       </c>
       <c r="H27" t="n">
-        <v>6301.32</v>
+        <v>6314.15</v>
       </c>
       <c r="I27" t="n">
-        <v>9398.59</v>
+        <v>9452.41</v>
       </c>
       <c r="J27" t="n">
-        <v>20312</v>
+        <v>20483</v>
       </c>
       <c r="K27" t="n">
-        <v>6301.32</v>
+        <v>6314.15</v>
       </c>
       <c r="L27" t="n">
-        <v>9398.59</v>
+        <v>9452.41</v>
       </c>
       <c r="M27" t="n">
         <v>1</v>
@@ -8892,22 +8892,22 @@
         <v>1</v>
       </c>
       <c r="G28" t="n">
-        <v>0.0001347</v>
+        <v>0.0001337</v>
       </c>
       <c r="H28" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="I28" t="n">
-        <v>59174.67</v>
+        <v>59068.31</v>
       </c>
       <c r="J28" t="n">
-        <v>134692</v>
+        <v>133707</v>
       </c>
       <c r="K28" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="L28" t="n">
-        <v>59174.67</v>
+        <v>59068.31</v>
       </c>
       <c r="M28" t="n">
         <v>1</v>
@@ -8945,22 +8945,22 @@
         <v>1</v>
       </c>
       <c r="G29" t="n">
-        <v>2.046e-05</v>
+        <v>2.067e-05</v>
       </c>
       <c r="H29" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="I29" t="n">
-        <v>18773.74</v>
+        <v>18886.56</v>
       </c>
       <c r="J29" t="n">
-        <v>20262</v>
+        <v>20468</v>
       </c>
       <c r="K29" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="L29" t="n">
-        <v>18773.74</v>
+        <v>18886.56</v>
       </c>
       <c r="M29" t="n">
         <v>1</v>
@@ -9001,7 +9001,7 @@
         <v>1.243e-05</v>
       </c>
       <c r="H30" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="I30" t="n">
         <v>12272.48</v>
@@ -9010,7 +9010,7 @@
         <v>12434</v>
       </c>
       <c r="K30" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="L30" t="n">
         <v>12272.48</v>
@@ -9051,22 +9051,22 @@
         <v>1</v>
       </c>
       <c r="G31" t="n">
-        <v>1.276e-05</v>
+        <v>1.299e-05</v>
       </c>
       <c r="H31" t="n">
-        <v>2590.53</v>
+        <v>2697.91</v>
       </c>
       <c r="I31" t="n">
-        <v>15027.69</v>
+        <v>15181.74</v>
       </c>
       <c r="J31" t="n">
-        <v>12730</v>
+        <v>12959</v>
       </c>
       <c r="K31" t="n">
-        <v>2590.53</v>
+        <v>2697.91</v>
       </c>
       <c r="L31" t="n">
-        <v>15027.69</v>
+        <v>15181.74</v>
       </c>
       <c r="M31" t="n">
         <v>1</v>
@@ -9107,7 +9107,7 @@
         <v>2.155e-05</v>
       </c>
       <c r="H32" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="I32" t="n">
         <v>19038.67</v>
@@ -9116,7 +9116,7 @@
         <v>21443</v>
       </c>
       <c r="K32" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="L32" t="n">
         <v>19038.67</v>
@@ -9187,17 +9187,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
+          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>IDIOT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>IDIOT</t>
         </is>
       </c>
       <c r="D34" s="2" t="n">
@@ -9210,22 +9210,22 @@
         <v>1</v>
       </c>
       <c r="G34" t="n">
-        <v>1649.46</v>
+        <v>2.909e-05</v>
       </c>
       <c r="H34" t="n">
-        <v>2288.31</v>
+        <v>2431.43</v>
       </c>
       <c r="I34" t="n">
-        <v>14828.26</v>
+        <v>23502.49</v>
       </c>
       <c r="J34" t="n">
-        <v>26638843</v>
+        <v>29094</v>
       </c>
       <c r="K34" t="n">
-        <v>2288.31</v>
+        <v>2431.43</v>
       </c>
       <c r="L34" t="n">
-        <v>14828.26</v>
+        <v>23502.49</v>
       </c>
       <c r="M34" t="n">
         <v>1</v>
@@ -9240,17 +9240,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
+          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RWA</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Real World Asses</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D35" s="2" t="n">
@@ -9263,22 +9263,22 @@
         <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>9.666000000000001e-08</v>
+        <v>1646.86</v>
       </c>
       <c r="H35" t="n">
-        <v>2243.13</v>
+        <v>2306.05</v>
       </c>
       <c r="I35" t="n">
-        <v>9081.24</v>
+        <v>14826.8</v>
       </c>
       <c r="J35" t="n">
-        <v>6670</v>
+        <v>26596804</v>
       </c>
       <c r="K35" t="n">
-        <v>2243.13</v>
+        <v>2306.05</v>
       </c>
       <c r="L35" t="n">
-        <v>9081.24</v>
+        <v>14826.8</v>
       </c>
       <c r="M35" t="n">
         <v>1</v>
@@ -9293,17 +9293,17 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
+          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>IDIOT</t>
+          <t>RWA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>IDIOT</t>
+          <t>Real World Asses</t>
         </is>
       </c>
       <c r="D36" s="2" t="n">
@@ -9316,22 +9316,22 @@
         <v>1</v>
       </c>
       <c r="G36" t="n">
-        <v>2.942e-05</v>
+        <v>9.504999999999999e-08</v>
       </c>
       <c r="H36" t="n">
-        <v>1830.81</v>
+        <v>2279.84</v>
       </c>
       <c r="I36" t="n">
-        <v>23157.24</v>
+        <v>9007.809999999999</v>
       </c>
       <c r="J36" t="n">
-        <v>29426</v>
+        <v>6559</v>
       </c>
       <c r="K36" t="n">
-        <v>1830.81</v>
+        <v>2279.84</v>
       </c>
       <c r="L36" t="n">
-        <v>23157.24</v>
+        <v>9007.809999999999</v>
       </c>
       <c r="M36" t="n">
         <v>1</v>
@@ -9369,22 +9369,22 @@
         <v>1</v>
       </c>
       <c r="G37" t="n">
-        <v>2.993e-05</v>
+        <v>2.96e-05</v>
       </c>
       <c r="H37" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="I37" t="n">
-        <v>21480.66</v>
+        <v>21416.84</v>
       </c>
       <c r="J37" t="n">
-        <v>29934</v>
+        <v>29604</v>
       </c>
       <c r="K37" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="L37" t="n">
-        <v>21480.66</v>
+        <v>21416.84</v>
       </c>
       <c r="M37" t="n">
         <v>1</v>
@@ -9475,22 +9475,22 @@
         <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>1.04e-05</v>
+        <v>1.036e-05</v>
       </c>
       <c r="H39" t="n">
-        <v>1355.84</v>
+        <v>1376.56</v>
       </c>
       <c r="I39" t="n">
-        <v>13484.99</v>
+        <v>13472.6</v>
       </c>
       <c r="J39" t="n">
-        <v>10409</v>
+        <v>10363</v>
       </c>
       <c r="K39" t="n">
-        <v>1355.84</v>
+        <v>1376.56</v>
       </c>
       <c r="L39" t="n">
-        <v>13484.99</v>
+        <v>13472.6</v>
       </c>
       <c r="M39" t="n">
         <v>1</v>
@@ -9528,22 +9528,22 @@
         <v>1</v>
       </c>
       <c r="G40" t="n">
-        <v>2.259e-05</v>
+        <v>2.326e-05</v>
       </c>
       <c r="H40" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="I40" t="n">
-        <v>22300.62</v>
+        <v>23013.57</v>
       </c>
       <c r="J40" t="n">
-        <v>22594</v>
+        <v>23265</v>
       </c>
       <c r="K40" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="L40" t="n">
-        <v>22300.62</v>
+        <v>23013.57</v>
       </c>
       <c r="M40" t="n">
         <v>1</v>
@@ -10088,17 +10088,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>9NcUwy9JVekfsY4UA62ZaTprn4TDnJZwp5B6vMAAtkzt</t>
+          <t>4CBToKTRKfBsv8RMfzMr6VfKQ8PLRYeG6RFGZmq4pump</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FLY</t>
+          <t>grandma</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Nexa</t>
+          <t>101 Year Old Pumpfun Livestreamr</t>
         </is>
       </c>
       <c r="D51" s="2" t="n">
@@ -10111,22 +10111,22 @@
         <v>1</v>
       </c>
       <c r="G51" t="n">
-        <v>0.01399</v>
+        <v>1.323e-05</v>
       </c>
       <c r="H51" t="n">
-        <v>45.53</v>
+        <v>54.86</v>
       </c>
       <c r="I51" t="n">
-        <v>8095.6</v>
+        <v>16735.19</v>
       </c>
       <c r="J51" t="n">
-        <v>13996</v>
+        <v>13005</v>
       </c>
       <c r="K51" t="n">
-        <v>45.53</v>
+        <v>54.86</v>
       </c>
       <c r="L51" t="n">
-        <v>8095.6</v>
+        <v>16735.19</v>
       </c>
       <c r="M51" t="n">
         <v>1</v>
@@ -10351,13 +10351,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>217.3</v>
+        <v>217.67</v>
       </c>
       <c r="F2" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="G2" t="n">
-        <v>55068304.14</v>
+        <v>55374839.99</v>
       </c>
       <c r="H2" t="n">
         <v>0</v>
@@ -10398,16 +10398,16 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.0001467</v>
+        <v>0.0001641</v>
       </c>
       <c r="F3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="G3" t="n">
-        <v>79895.31</v>
+        <v>83232.7</v>
       </c>
       <c r="H3" t="n">
-        <v>146749</v>
+        <v>164163</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -10445,16 +10445,16 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.001647</v>
+        <v>0.0016</v>
       </c>
       <c r="F4" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="G4" t="n">
-        <v>224085.03</v>
+        <v>221116.95</v>
       </c>
       <c r="H4" t="n">
-        <v>1280147</v>
+        <v>1244218</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -10492,16 +10492,16 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.002688</v>
+        <v>0.00269</v>
       </c>
       <c r="F5" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="G5" t="n">
-        <v>500882.98</v>
+        <v>501076.47</v>
       </c>
       <c r="H5" t="n">
-        <v>2686803</v>
+        <v>2688607</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -10539,16 +10539,16 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.0004236</v>
+        <v>0.0004245</v>
       </c>
       <c r="F6" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="G6" t="n">
-        <v>124024.45</v>
+        <v>124317.64</v>
       </c>
       <c r="H6" t="n">
-        <v>423594</v>
+        <v>424479</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -10586,16 +10586,16 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.0001839</v>
+        <v>0.0001816</v>
       </c>
       <c r="F7" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="G7" t="n">
-        <v>53759.6</v>
+        <v>53430.12</v>
       </c>
       <c r="H7" t="n">
-        <v>183981</v>
+        <v>181694</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -10633,16 +10633,16 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0.0008705</v>
+        <v>0.0008823</v>
       </c>
       <c r="F8" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="G8" t="n">
-        <v>199804.55</v>
+        <v>201193.35</v>
       </c>
       <c r="H8" t="n">
-        <v>870510</v>
+        <v>882390</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -10680,16 +10680,16 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.001813</v>
+        <v>0.001829</v>
       </c>
       <c r="F9" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="G9" t="n">
-        <v>189799.17</v>
+        <v>190853.78</v>
       </c>
       <c r="H9" t="n">
-        <v>1813152</v>
+        <v>1829689</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -10730,7 +10730,7 @@
         <v>0.0002214</v>
       </c>
       <c r="F10" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="G10" t="n">
         <v>58993.73</v>
@@ -10774,16 +10774,16 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.01617</v>
+        <v>0.01623</v>
       </c>
       <c r="F11" t="n">
-        <v>83707.00999999999</v>
+        <v>82202</v>
       </c>
       <c r="G11" t="n">
-        <v>2105164.95</v>
+        <v>2110607.3</v>
       </c>
       <c r="H11" t="n">
-        <v>80878379</v>
+        <v>81173576</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -10824,7 +10824,7 @@
         <v>0.00111</v>
       </c>
       <c r="F12" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="G12" t="n">
         <v>166013.41</v>
@@ -10871,7 +10871,7 @@
         <v>0.0006933</v>
       </c>
       <c r="F13" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="G13" t="n">
         <v>104294.04</v>
@@ -10915,16 +10915,16 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.0004602</v>
+        <v>0.0004622</v>
       </c>
       <c r="F14" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="G14" t="n">
-        <v>138294.92</v>
+        <v>138661.32</v>
       </c>
       <c r="H14" t="n">
-        <v>460190</v>
+        <v>462204</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -10962,16 +10962,16 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.0002183</v>
+        <v>0.0002218</v>
       </c>
       <c r="F15" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="G15" t="n">
-        <v>74040.59</v>
+        <v>74592.92999999999</v>
       </c>
       <c r="H15" t="n">
-        <v>217631</v>
+        <v>221086</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -11009,16 +11009,16 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.0005199</v>
+        <v>0.0005284000000000001</v>
       </c>
       <c r="F16" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="G16" t="n">
-        <v>148065.02</v>
+        <v>149501</v>
       </c>
       <c r="H16" t="n">
-        <v>519796</v>
+        <v>528322</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -11059,7 +11059,7 @@
         <v>0.000112</v>
       </c>
       <c r="F17" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="G17" t="n">
         <v>56740.29</v>
@@ -11103,16 +11103,16 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.0003056</v>
+        <v>0.0003025</v>
       </c>
       <c r="F18" t="n">
-        <v>38198.12</v>
+        <v>39570.21</v>
       </c>
       <c r="G18" t="n">
-        <v>72990.33</v>
+        <v>72811.57000000001</v>
       </c>
       <c r="H18" t="n">
-        <v>305574</v>
+        <v>302512</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -11150,16 +11150,16 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.0004733</v>
+        <v>0.0004963</v>
       </c>
       <c r="F19" t="n">
-        <v>31601.34</v>
+        <v>35912.32</v>
       </c>
       <c r="G19" t="n">
-        <v>175629.27</v>
+        <v>180047.48</v>
       </c>
       <c r="H19" t="n">
-        <v>473325</v>
+        <v>496394</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -11197,16 +11197,16 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>6.745999999999999e-05</v>
+        <v>6.567999999999999e-05</v>
       </c>
       <c r="F20" t="n">
-        <v>18225.35</v>
+        <v>18606.34</v>
       </c>
       <c r="G20" t="n">
-        <v>39289.74</v>
+        <v>38871.85</v>
       </c>
       <c r="H20" t="n">
-        <v>67461</v>
+        <v>65683</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -11230,30 +11230,30 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>VIBECODER</t>
+          <t>walkusa</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Vibe Coding Meta</t>
+          <t>WALKING ACROSS AMERICA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.0001341</v>
+        <v>7.773e-05</v>
       </c>
       <c r="F21" t="n">
-        <v>17344.55</v>
+        <v>17207.7</v>
       </c>
       <c r="G21" t="n">
-        <v>53854.17</v>
+        <v>38711.88</v>
       </c>
       <c r="H21" t="n">
-        <v>130146</v>
+        <v>77734</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -11277,30 +11277,30 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>walkusa</t>
+          <t>VIBECODER</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>WALKING ACROSS AMERICA</t>
+          <t>Vibe Coding Meta</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3BrXeqzNKUKsM6MgkWFZX4E2cY8SiwYNwwmVzP2Rpump</t>
+          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>7.773e-05</v>
+        <v>0.0001341</v>
       </c>
       <c r="F22" t="n">
-        <v>17207.7</v>
+        <v>17176.84</v>
       </c>
       <c r="G22" t="n">
-        <v>38711.88</v>
+        <v>53854.17</v>
       </c>
       <c r="H22" t="n">
-        <v>77734</v>
+        <v>130146</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
@@ -11341,7 +11341,7 @@
         <v>6.069e-05</v>
       </c>
       <c r="F23" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="G23" t="n">
         <v>31664.06</v>
@@ -11435,7 +11435,7 @@
         <v>0.000151</v>
       </c>
       <c r="F25" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="G25" t="n">
         <v>86166.2</v>
@@ -11479,16 +11479,16 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.003955</v>
+        <v>0.003962</v>
       </c>
       <c r="F26" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="G26" t="n">
-        <v>574364.5</v>
+        <v>576259.42</v>
       </c>
       <c r="H26" t="n">
-        <v>3955131</v>
+        <v>3962041</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -11526,16 +11526,16 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2.031e-05</v>
+        <v>2.048e-05</v>
       </c>
       <c r="F27" t="n">
-        <v>6301.32</v>
+        <v>6314.15</v>
       </c>
       <c r="G27" t="n">
-        <v>9398.59</v>
+        <v>9452.41</v>
       </c>
       <c r="H27" t="n">
-        <v>20312</v>
+        <v>20483</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
@@ -11573,16 +11573,16 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.0001347</v>
+        <v>0.0001337</v>
       </c>
       <c r="F28" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="G28" t="n">
-        <v>59174.67</v>
+        <v>59068.31</v>
       </c>
       <c r="H28" t="n">
-        <v>134692</v>
+        <v>133707</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -11620,16 +11620,16 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2.046e-05</v>
+        <v>2.067e-05</v>
       </c>
       <c r="F29" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="G29" t="n">
-        <v>18773.74</v>
+        <v>18886.56</v>
       </c>
       <c r="H29" t="n">
-        <v>20262</v>
+        <v>20468</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -11670,7 +11670,7 @@
         <v>1.243e-05</v>
       </c>
       <c r="F30" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="G30" t="n">
         <v>12272.48</v>
@@ -11714,16 +11714,16 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>1.276e-05</v>
+        <v>1.299e-05</v>
       </c>
       <c r="F31" t="n">
-        <v>2590.53</v>
+        <v>2697.91</v>
       </c>
       <c r="G31" t="n">
-        <v>15027.69</v>
+        <v>15181.74</v>
       </c>
       <c r="H31" t="n">
-        <v>12730</v>
+        <v>12959</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -11764,7 +11764,7 @@
         <v>2.155e-05</v>
       </c>
       <c r="F32" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="G32" t="n">
         <v>19038.67</v>
@@ -11841,30 +11841,30 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>SOL</t>
+          <t>IDIOT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Solana</t>
+          <t>IDIOT</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
+          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>1649.46</v>
+        <v>2.909e-05</v>
       </c>
       <c r="F34" t="n">
-        <v>2288.31</v>
+        <v>2431.43</v>
       </c>
       <c r="G34" t="n">
-        <v>14828.26</v>
+        <v>23502.49</v>
       </c>
       <c r="H34" t="n">
-        <v>26638843</v>
+        <v>29094</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -11888,30 +11888,30 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RWA</t>
+          <t>SOL</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Real World Asses</t>
+          <t>Solana</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
+          <t>9n4nbM75f5Ui33ZbPYXn59EwSgE8CGsHtAeTH5YFeJ9E</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>9.666000000000001e-08</v>
+        <v>1646.86</v>
       </c>
       <c r="F35" t="n">
-        <v>2243.13</v>
+        <v>2306.05</v>
       </c>
       <c r="G35" t="n">
-        <v>9081.24</v>
+        <v>14826.8</v>
       </c>
       <c r="H35" t="n">
-        <v>6670</v>
+        <v>26596804</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -11935,30 +11935,30 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>IDIOT</t>
+          <t>RWA</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>IDIOT</t>
+          <t>Real World Asses</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>GcPf1ZsZHvnjauhXoFvGMmc2gM73aJ63AYxYC6JAQVoG</t>
+          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>2.942e-05</v>
+        <v>9.504999999999999e-08</v>
       </c>
       <c r="F36" t="n">
-        <v>1830.81</v>
+        <v>2279.84</v>
       </c>
       <c r="G36" t="n">
-        <v>23157.24</v>
+        <v>9007.809999999999</v>
       </c>
       <c r="H36" t="n">
-        <v>29426</v>
+        <v>6559</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -11996,16 +11996,16 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>2.993e-05</v>
+        <v>2.96e-05</v>
       </c>
       <c r="F37" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="G37" t="n">
-        <v>21480.66</v>
+        <v>21416.84</v>
       </c>
       <c r="H37" t="n">
-        <v>29934</v>
+        <v>29604</v>
       </c>
       <c r="I37" t="inlineStr">
         <is>
@@ -12090,16 +12090,16 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>1.04e-05</v>
+        <v>1.036e-05</v>
       </c>
       <c r="F39" t="n">
-        <v>1355.84</v>
+        <v>1376.56</v>
       </c>
       <c r="G39" t="n">
-        <v>13484.99</v>
+        <v>13472.6</v>
       </c>
       <c r="H39" t="n">
-        <v>10409</v>
+        <v>10363</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -12137,16 +12137,16 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>2.259e-05</v>
+        <v>2.326e-05</v>
       </c>
       <c r="F40" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="G40" t="n">
-        <v>22300.62</v>
+        <v>23013.57</v>
       </c>
       <c r="H40" t="n">
-        <v>22594</v>
+        <v>23265</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -12640,30 +12640,30 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>FLY</t>
+          <t>grandma</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Nexa</t>
+          <t>101 Year Old Pumpfun Livestreamr</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>9NcUwy9JVekfsY4UA62ZaTprn4TDnJZwp5B6vMAAtkzt</t>
+          <t>4CBToKTRKfBsv8RMfzMr6VfKQ8PLRYeG6RFGZmq4pump</t>
         </is>
       </c>
       <c r="E51" t="n">
-        <v>0.01399</v>
+        <v>1.323e-05</v>
       </c>
       <c r="F51" t="n">
-        <v>45.53</v>
+        <v>54.86</v>
       </c>
       <c r="G51" t="n">
-        <v>8095.6</v>
+        <v>16735.19</v>
       </c>
       <c r="H51" t="n">
-        <v>13996</v>
+        <v>13005</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -15674,25 +15674,25 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="E2" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="F2" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="G2" t="n">
-        <v>4576.76</v>
+        <v>4616.94</v>
       </c>
       <c r="H2" t="n">
-        <v>18773.74</v>
+        <v>18886.56</v>
       </c>
       <c r="I2" t="n">
-        <v>18773.74</v>
+        <v>18886.56</v>
       </c>
       <c r="J2" t="n">
-        <v>18773.74</v>
+        <v>18886.56</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
@@ -15725,25 +15725,25 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="E3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="F3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="G3" t="n">
-        <v>983529.58</v>
+        <v>979398.59</v>
       </c>
       <c r="H3" t="n">
-        <v>79895.31</v>
+        <v>83232.7</v>
       </c>
       <c r="I3" t="n">
-        <v>79895.31</v>
+        <v>83232.7</v>
       </c>
       <c r="J3" t="n">
-        <v>79895.31</v>
+        <v>83232.7</v>
       </c>
       <c r="K3" t="n">
         <v>1</v>
@@ -15776,16 +15776,16 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="E4" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="F4" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="G4" t="n">
-        <v>41114.17</v>
+        <v>41053.76</v>
       </c>
       <c r="H4" t="n">
         <v>56740.29</v>
@@ -15878,25 +15878,25 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="E6" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="F6" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="G6" t="n">
-        <v>7170.72</v>
+        <v>7551.98</v>
       </c>
       <c r="H6" t="n">
-        <v>574364.5</v>
+        <v>576259.42</v>
       </c>
       <c r="I6" t="n">
-        <v>574364.5</v>
+        <v>576259.42</v>
       </c>
       <c r="J6" t="n">
-        <v>574364.5</v>
+        <v>576259.42</v>
       </c>
       <c r="K6" t="n">
         <v>1</v>
@@ -15929,25 +15929,25 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="E7" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="F7" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="G7" t="n">
-        <v>52562.9</v>
+        <v>52987.33</v>
       </c>
       <c r="H7" t="n">
-        <v>148065.02</v>
+        <v>149501</v>
       </c>
       <c r="I7" t="n">
-        <v>148065.02</v>
+        <v>149501</v>
       </c>
       <c r="J7" t="n">
-        <v>148065.02</v>
+        <v>149501</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
@@ -15980,25 +15980,25 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="E8" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="F8" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="G8" t="n">
-        <v>149172.78</v>
+        <v>151000.53</v>
       </c>
       <c r="H8" t="n">
-        <v>53759.6</v>
+        <v>53430.12</v>
       </c>
       <c r="I8" t="n">
-        <v>53759.6</v>
+        <v>53430.12</v>
       </c>
       <c r="J8" t="n">
-        <v>53759.6</v>
+        <v>53430.12</v>
       </c>
       <c r="K8" t="n">
         <v>1</v>
@@ -16022,34 +16022,34 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4bLnK5YuJaqkVX4uWtJ1Qtx3XoZ8eHH37STXSwujpump</t>
+          <t>4CBToKTRKfBsv8RMfzMr6VfKQ8PLRYeG6RFGZmq4pump</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>DARE</t>
+          <t>grandma</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>649.3</v>
+        <v>54.86</v>
       </c>
       <c r="E9" t="n">
-        <v>649.3</v>
+        <v>54.86</v>
       </c>
       <c r="F9" t="n">
-        <v>649.3</v>
+        <v>54.86</v>
       </c>
       <c r="G9" t="n">
-        <v>649.3</v>
+        <v>54.86</v>
       </c>
       <c r="H9" t="n">
-        <v>13436.27</v>
+        <v>16735.19</v>
       </c>
       <c r="I9" t="n">
-        <v>13436.27</v>
+        <v>16735.19</v>
       </c>
       <c r="J9" t="n">
-        <v>13436.27</v>
+        <v>16735.19</v>
       </c>
       <c r="K9" t="n">
         <v>1</v>
@@ -16073,34 +16073,34 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4ky1REfghVawQ6EPZGdx7zss5KNKStwE8swjii3uU5sD</t>
+          <t>4bLnK5YuJaqkVX4uWtJ1Qtx3XoZ8eHH37STXSwujpump</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MOCHI</t>
+          <t>DARE</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1592.82</v>
+        <v>649.3</v>
       </c>
       <c r="E10" t="n">
-        <v>1592.82</v>
+        <v>649.3</v>
       </c>
       <c r="F10" t="n">
-        <v>1592.82</v>
+        <v>649.3</v>
       </c>
       <c r="G10" t="n">
-        <v>1592.82</v>
+        <v>649.3</v>
       </c>
       <c r="H10" t="n">
-        <v>24287.67</v>
+        <v>13436.27</v>
       </c>
       <c r="I10" t="n">
-        <v>24287.67</v>
+        <v>13436.27</v>
       </c>
       <c r="J10" t="n">
-        <v>24287.67</v>
+        <v>13436.27</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
@@ -16124,34 +16124,34 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
+          <t>4ky1REfghVawQ6EPZGdx7zss5KNKStwE8swjii3uU5sD</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Useless</t>
+          <t>MOCHI</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>18225.35</v>
+        <v>1592.82</v>
       </c>
       <c r="E11" t="n">
-        <v>18225.35</v>
+        <v>1592.82</v>
       </c>
       <c r="F11" t="n">
-        <v>18225.35</v>
+        <v>1592.82</v>
       </c>
       <c r="G11" t="n">
-        <v>18225.35</v>
+        <v>1592.82</v>
       </c>
       <c r="H11" t="n">
-        <v>39289.74</v>
+        <v>24287.67</v>
       </c>
       <c r="I11" t="n">
-        <v>39289.74</v>
+        <v>24287.67</v>
       </c>
       <c r="J11" t="n">
-        <v>39289.74</v>
+        <v>24287.67</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
@@ -16175,34 +16175,34 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6FtbGaqgZzti1TxJksBV4PSya5of9VqA9vJNDxPwbonk</t>
+          <t>5NnL7oRMtVW3ZqAt95gJQs12Fbz2caCYh9rgy1kQpump</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>gib</t>
+          <t>Useless</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>31601.34</v>
+        <v>18606.34</v>
       </c>
       <c r="E12" t="n">
-        <v>31601.34</v>
+        <v>18606.34</v>
       </c>
       <c r="F12" t="n">
-        <v>31601.34</v>
+        <v>18606.34</v>
       </c>
       <c r="G12" t="n">
-        <v>31601.34</v>
+        <v>18606.34</v>
       </c>
       <c r="H12" t="n">
-        <v>175629.27</v>
+        <v>38871.85</v>
       </c>
       <c r="I12" t="n">
-        <v>175629.27</v>
+        <v>38871.85</v>
       </c>
       <c r="J12" t="n">
-        <v>175629.27</v>
+        <v>38871.85</v>
       </c>
       <c r="K12" t="n">
         <v>1</v>
@@ -16226,34 +16226,34 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>6NVo6X8ouYRVoKRWe7Y9J6CT4pWZXDthSJCBZ3vgUg8z</t>
+          <t>6FtbGaqgZzti1TxJksBV4PSya5of9VqA9vJNDxPwbonk</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Bagwork</t>
+          <t>gib</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>114.4</v>
+        <v>35912.32</v>
       </c>
       <c r="E13" t="n">
-        <v>114.4</v>
+        <v>35912.32</v>
       </c>
       <c r="F13" t="n">
-        <v>114.4</v>
+        <v>35912.32</v>
       </c>
       <c r="G13" t="n">
-        <v>114.4</v>
+        <v>35912.32</v>
       </c>
       <c r="H13" t="n">
-        <v>8930.35</v>
+        <v>180047.48</v>
       </c>
       <c r="I13" t="n">
-        <v>8930.35</v>
+        <v>180047.48</v>
       </c>
       <c r="J13" t="n">
-        <v>8930.35</v>
+        <v>180047.48</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>
@@ -16277,34 +16277,34 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
+          <t>6NVo6X8ouYRVoKRWe7Y9J6CT4pWZXDthSJCBZ3vgUg8z</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>retail</t>
+          <t>Bagwork</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>134.48</v>
+        <v>114.4</v>
       </c>
       <c r="E14" t="n">
-        <v>134.48</v>
+        <v>114.4</v>
       </c>
       <c r="F14" t="n">
-        <v>134.48</v>
+        <v>114.4</v>
       </c>
       <c r="G14" t="n">
-        <v>134.48</v>
+        <v>114.4</v>
       </c>
       <c r="H14" t="n">
-        <v>8042.59</v>
+        <v>8930.35</v>
       </c>
       <c r="I14" t="n">
-        <v>8042.59</v>
+        <v>8930.35</v>
       </c>
       <c r="J14" t="n">
-        <v>8042.59</v>
+        <v>8930.35</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
@@ -16328,34 +16328,34 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>6k1rwsNMBwbRJrWck3sEVCjn4MvF9ty8A6iSGfxjxREV</t>
+          <t>6jPg6gSrwtJyHWGTs7tUh2Zs1GzfKzHQNUGfAK1xpump</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>APOLLO</t>
+          <t>retail</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>6301.32</v>
+        <v>134.48</v>
       </c>
       <c r="E15" t="n">
-        <v>6301.32</v>
+        <v>134.48</v>
       </c>
       <c r="F15" t="n">
-        <v>6301.32</v>
+        <v>134.48</v>
       </c>
       <c r="G15" t="n">
-        <v>6301.32</v>
+        <v>134.48</v>
       </c>
       <c r="H15" t="n">
-        <v>9398.59</v>
+        <v>8042.59</v>
       </c>
       <c r="I15" t="n">
-        <v>9398.59</v>
+        <v>8042.59</v>
       </c>
       <c r="J15" t="n">
-        <v>9398.59</v>
+        <v>8042.59</v>
       </c>
       <c r="K15" t="n">
         <v>1</v>
@@ -16379,34 +16379,34 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
+          <t>6k1rwsNMBwbRJrWck3sEVCjn4MvF9ty8A6iSGfxjxREV</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>RWA</t>
+          <t>APOLLO</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>2243.13</v>
+        <v>6314.15</v>
       </c>
       <c r="E16" t="n">
-        <v>2243.13</v>
+        <v>6314.15</v>
       </c>
       <c r="F16" t="n">
-        <v>2243.13</v>
+        <v>6314.15</v>
       </c>
       <c r="G16" t="n">
-        <v>2243.13</v>
+        <v>6314.15</v>
       </c>
       <c r="H16" t="n">
-        <v>9081.24</v>
+        <v>9452.41</v>
       </c>
       <c r="I16" t="n">
-        <v>9081.24</v>
+        <v>9452.41</v>
       </c>
       <c r="J16" t="n">
-        <v>9081.24</v>
+        <v>9452.41</v>
       </c>
       <c r="K16" t="n">
         <v>1</v>
@@ -16430,34 +16430,34 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
+          <t>7N8qk43L1PCcaqudkEasGpKqcunX1ChXYo2VB1g8bonk</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>VIBECODER</t>
+          <t>RWA</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>17344.55</v>
+        <v>2279.84</v>
       </c>
       <c r="E17" t="n">
-        <v>17344.55</v>
+        <v>2279.84</v>
       </c>
       <c r="F17" t="n">
-        <v>17344.55</v>
+        <v>2279.84</v>
       </c>
       <c r="G17" t="n">
-        <v>17344.55</v>
+        <v>2279.84</v>
       </c>
       <c r="H17" t="n">
-        <v>53854.17</v>
+        <v>9007.809999999999</v>
       </c>
       <c r="I17" t="n">
-        <v>53854.17</v>
+        <v>9007.809999999999</v>
       </c>
       <c r="J17" t="n">
-        <v>53854.17</v>
+        <v>9007.809999999999</v>
       </c>
       <c r="K17" t="n">
         <v>1</v>
@@ -16481,34 +16481,34 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>7kN5FQMD8ja4bzysEgc5FXmryKd6gCgjiWnhksjHCFb3</t>
+          <t>7PzU4m13VqkdgWcserfBdxX4cAPQXaZuFNuKarnT1deV</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>LION</t>
+          <t>VIBECODER</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>83707.00999999999</v>
+        <v>17176.84</v>
       </c>
       <c r="E18" t="n">
-        <v>83707.00999999999</v>
+        <v>17176.84</v>
       </c>
       <c r="F18" t="n">
-        <v>83707.00999999999</v>
+        <v>17176.84</v>
       </c>
       <c r="G18" t="n">
-        <v>83707.00999999999</v>
+        <v>17176.84</v>
       </c>
       <c r="H18" t="n">
-        <v>2105164.95</v>
+        <v>53854.17</v>
       </c>
       <c r="I18" t="n">
-        <v>2105164.95</v>
+        <v>53854.17</v>
       </c>
       <c r="J18" t="n">
-        <v>2105164.95</v>
+        <v>53854.17</v>
       </c>
       <c r="K18" t="n">
         <v>1</v>
@@ -16532,34 +16532,34 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>7ukFzJA7V6f28YieCjXcEXqiK8tAfbyXyvK6b36pump</t>
+          <t>7kN5FQMD8ja4bzysEgc5FXmryKd6gCgjiWnhksjHCFb3</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>early</t>
+          <t>LION</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>38198.12</v>
+        <v>82202</v>
       </c>
       <c r="E19" t="n">
-        <v>38198.12</v>
+        <v>82202</v>
       </c>
       <c r="F19" t="n">
-        <v>38198.12</v>
+        <v>82202</v>
       </c>
       <c r="G19" t="n">
-        <v>38198.12</v>
+        <v>82202</v>
       </c>
       <c r="H19" t="n">
-        <v>72990.33</v>
+        <v>2110607.3</v>
       </c>
       <c r="I19" t="n">
-        <v>72990.33</v>
+        <v>2110607.3</v>
       </c>
       <c r="J19" t="n">
-        <v>72990.33</v>
+        <v>2110607.3</v>
       </c>
       <c r="K19" t="n">
         <v>1</v>
@@ -16583,34 +16583,34 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>8erRtd8mLgNcNoWy2bhMdTgZyXaRR6u7t2hyXRc1pump</t>
+          <t>7ukFzJA7V6f28YieCjXcEXqiK8tAfbyXyvK6b36pump</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1dog</t>
+          <t>early</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>2590.53</v>
+        <v>39570.21</v>
       </c>
       <c r="E20" t="n">
-        <v>2590.53</v>
+        <v>39570.21</v>
       </c>
       <c r="F20" t="n">
-        <v>2590.53</v>
+        <v>39570.21</v>
       </c>
       <c r="G20" t="n">
-        <v>2590.53</v>
+        <v>39570.21</v>
       </c>
       <c r="H20" t="n">
-        <v>15027.69</v>
+        <v>72811.57000000001</v>
       </c>
       <c r="I20" t="n">
-        <v>15027.69</v>
+        <v>72811.57000000001</v>
       </c>
       <c r="J20" t="n">
-        <v>15027.69</v>
+        <v>72811.57000000001</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
@@ -16634,34 +16634,34 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>8wbfBYthc9fC4GsHgCtznZP1PAoXaZ8tnUGBtGMgpump</t>
+          <t>8erRtd8mLgNcNoWy2bhMdTgZyXaRR6u7t2hyXRc1pump</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>1dog</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2456.3</v>
+        <v>2697.91</v>
       </c>
       <c r="E21" t="n">
-        <v>2456.3</v>
+        <v>2697.91</v>
       </c>
       <c r="F21" t="n">
-        <v>2456.3</v>
+        <v>2697.91</v>
       </c>
       <c r="G21" t="n">
-        <v>2456.3</v>
+        <v>2697.91</v>
       </c>
       <c r="H21" t="n">
-        <v>11616.2</v>
+        <v>15181.74</v>
       </c>
       <c r="I21" t="n">
-        <v>11616.2</v>
+        <v>15181.74</v>
       </c>
       <c r="J21" t="n">
-        <v>11616.2</v>
+        <v>15181.74</v>
       </c>
       <c r="K21" t="n">
         <v>1</v>
@@ -16685,34 +16685,34 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>8z55m3BmsPkmDfi5b5dAomBvYi1cDmW92hrEJTLdpump</t>
+          <t>8wbfBYthc9fC4GsHgCtznZP1PAoXaZ8tnUGBtGMgpump</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PILL</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>97.42</v>
+        <v>2456.3</v>
       </c>
       <c r="E22" t="n">
-        <v>97.42</v>
+        <v>2456.3</v>
       </c>
       <c r="F22" t="n">
-        <v>97.42</v>
+        <v>2456.3</v>
       </c>
       <c r="G22" t="n">
-        <v>97.42</v>
+        <v>2456.3</v>
       </c>
       <c r="H22" t="n">
-        <v>10687.28</v>
+        <v>11616.2</v>
       </c>
       <c r="I22" t="n">
-        <v>10687.28</v>
+        <v>11616.2</v>
       </c>
       <c r="J22" t="n">
-        <v>10687.28</v>
+        <v>11616.2</v>
       </c>
       <c r="K22" t="n">
         <v>1</v>
@@ -16736,34 +16736,34 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>99YFbXS6iA7s1qkRDTMBXEywtLNmrRtHtGKvNxpKWcdT</t>
+          <t>8z55m3BmsPkmDfi5b5dAomBvYi1cDmW92hrEJTLdpump</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MOON</t>
+          <t>PILL</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>1355.84</v>
+        <v>97.42</v>
       </c>
       <c r="E23" t="n">
-        <v>1355.84</v>
+        <v>97.42</v>
       </c>
       <c r="F23" t="n">
-        <v>1355.84</v>
+        <v>97.42</v>
       </c>
       <c r="G23" t="n">
-        <v>1355.84</v>
+        <v>97.42</v>
       </c>
       <c r="H23" t="n">
-        <v>13484.99</v>
+        <v>10687.28</v>
       </c>
       <c r="I23" t="n">
-        <v>13484.99</v>
+        <v>10687.28</v>
       </c>
       <c r="J23" t="n">
-        <v>13484.99</v>
+        <v>10687.28</v>
       </c>
       <c r="K23" t="n">
         <v>1</v>
@@ -16787,34 +16787,34 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>9NcUwy9JVekfsY4UA62ZaTprn4TDnJZwp5B6vMAAtkzt</t>
+          <t>99YFbXS6iA7s1qkRDTMBXEywtLNmrRtHtGKvNxpKWcdT</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>FLY</t>
+          <t>MOON</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>45.53</v>
+        <v>1376.56</v>
       </c>
       <c r="E24" t="n">
-        <v>45.53</v>
+        <v>1376.56</v>
       </c>
       <c r="F24" t="n">
-        <v>45.53</v>
+        <v>1376.56</v>
       </c>
       <c r="G24" t="n">
-        <v>45.53</v>
+        <v>1376.56</v>
       </c>
       <c r="H24" t="n">
-        <v>8095.6</v>
+        <v>13472.6</v>
       </c>
       <c r="I24" t="n">
-        <v>8095.6</v>
+        <v>13472.6</v>
       </c>
       <c r="J24" t="n">
-        <v>8095.6</v>
+        <v>13472.6</v>
       </c>
       <c r="K24" t="n">
         <v>1</v>
@@ -16847,25 +16847,25 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="E25" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="F25" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="G25" t="n">
-        <v>1065.96</v>
+        <v>1093.82</v>
       </c>
       <c r="H25" t="n">
-        <v>22300.62</v>
+        <v>23013.57</v>
       </c>
       <c r="I25" t="n">
-        <v>22300.62</v>
+        <v>23013.57</v>
       </c>
       <c r="J25" t="n">
-        <v>22300.62</v>
+        <v>23013.57</v>
       </c>
       <c r="K25" t="n">
         <v>1</v>
@@ -16898,25 +16898,25 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2288.31</v>
+        <v>2306.05</v>
       </c>
       <c r="E26" t="n">
-        <v>2288.31</v>
+        <v>2306.05</v>
       </c>
       <c r="F26" t="n">
-        <v>2288.31</v>
+        <v>2306.05</v>
       </c>
       <c r="G26" t="n">
-        <v>2288.31</v>
+        <v>2306.05</v>
       </c>
       <c r="H26" t="n">
-        <v>14828.26</v>
+        <v>14826.8</v>
       </c>
       <c r="I26" t="n">
-        <v>14828.26</v>
+        <v>14826.8</v>
       </c>
       <c r="J26" t="n">
-        <v>14828.26</v>
+        <v>14826.8</v>
       </c>
       <c r="K26" t="n">
         <v>1</v>
@@ -16949,16 +16949,16 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="E27" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="F27" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="G27" t="n">
-        <v>2578.38</v>
+        <v>2575.06</v>
       </c>
       <c r="H27" t="n">
         <v>19038.67</v>
@@ -17000,25 +17000,25 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="E28" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="F28" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="G28" t="n">
-        <v>271130.93</v>
+        <v>271917.29</v>
       </c>
       <c r="H28" t="n">
-        <v>500882.98</v>
+        <v>501076.47</v>
       </c>
       <c r="I28" t="n">
-        <v>500882.98</v>
+        <v>501076.47</v>
       </c>
       <c r="J28" t="n">
-        <v>500882.98</v>
+        <v>501076.47</v>
       </c>
       <c r="K28" t="n">
         <v>1</v>
@@ -17051,16 +17051,16 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="E29" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="F29" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="G29" t="n">
-        <v>66873.19</v>
+        <v>66691.25999999999</v>
       </c>
       <c r="H29" t="n">
         <v>104294.04</v>
@@ -17102,25 +17102,25 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="E30" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="F30" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="G30" t="n">
-        <v>95369</v>
+        <v>103303.9</v>
       </c>
       <c r="H30" t="n">
-        <v>189799.17</v>
+        <v>190853.78</v>
       </c>
       <c r="I30" t="n">
-        <v>189799.17</v>
+        <v>190853.78</v>
       </c>
       <c r="J30" t="n">
-        <v>189799.17</v>
+        <v>190853.78</v>
       </c>
       <c r="K30" t="n">
         <v>1</v>
@@ -17153,25 +17153,25 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="E31" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="F31" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="G31" t="n">
-        <v>60667.55</v>
+        <v>60840.08</v>
       </c>
       <c r="H31" t="n">
-        <v>74040.59</v>
+        <v>74592.92999999999</v>
       </c>
       <c r="I31" t="n">
-        <v>74040.59</v>
+        <v>74592.92999999999</v>
       </c>
       <c r="J31" t="n">
-        <v>74040.59</v>
+        <v>74592.92999999999</v>
       </c>
       <c r="K31" t="n">
         <v>1</v>
@@ -17204,25 +17204,25 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="E32" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="F32" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="G32" t="n">
-        <v>66287.08</v>
+        <v>65937.16</v>
       </c>
       <c r="H32" t="n">
-        <v>138294.92</v>
+        <v>138661.32</v>
       </c>
       <c r="I32" t="n">
-        <v>138294.92</v>
+        <v>138661.32</v>
       </c>
       <c r="J32" t="n">
-        <v>138294.92</v>
+        <v>138661.32</v>
       </c>
       <c r="K32" t="n">
         <v>1</v>
@@ -17255,25 +17255,25 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="E33" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="F33" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="G33" t="n">
-        <v>185500.61</v>
+        <v>185563.84</v>
       </c>
       <c r="H33" t="n">
-        <v>124024.45</v>
+        <v>124317.64</v>
       </c>
       <c r="I33" t="n">
-        <v>124024.45</v>
+        <v>124317.64</v>
       </c>
       <c r="J33" t="n">
-        <v>124024.45</v>
+        <v>124317.64</v>
       </c>
       <c r="K33" t="n">
         <v>1</v>
@@ -17357,25 +17357,25 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="E35" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="F35" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="G35" t="n">
-        <v>384087.91</v>
+        <v>383498.04</v>
       </c>
       <c r="H35" t="n">
-        <v>224085.03</v>
+        <v>221116.95</v>
       </c>
       <c r="I35" t="n">
-        <v>224085.03</v>
+        <v>221116.95</v>
       </c>
       <c r="J35" t="n">
-        <v>224085.03</v>
+        <v>221116.95</v>
       </c>
       <c r="K35" t="n">
         <v>1</v>
@@ -17408,16 +17408,16 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="E36" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="F36" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="G36" t="n">
-        <v>12642.5</v>
+        <v>11406.34</v>
       </c>
       <c r="H36" t="n">
         <v>31664.06</v>
@@ -17459,16 +17459,16 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="E37" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="F37" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="G37" t="n">
-        <v>91680.53</v>
+        <v>90657.73</v>
       </c>
       <c r="H37" t="n">
         <v>58993.73</v>
@@ -17612,25 +17612,25 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="E40" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="F40" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="G40" t="n">
-        <v>122406.18</v>
+        <v>122958.31</v>
       </c>
       <c r="H40" t="n">
-        <v>199804.55</v>
+        <v>201193.35</v>
       </c>
       <c r="I40" t="n">
-        <v>199804.55</v>
+        <v>201193.35</v>
       </c>
       <c r="J40" t="n">
-        <v>199804.55</v>
+        <v>201193.35</v>
       </c>
       <c r="K40" t="n">
         <v>1</v>
@@ -17663,16 +17663,16 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="E41" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="F41" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="G41" t="n">
-        <v>4123.8</v>
+        <v>3906.88</v>
       </c>
       <c r="H41" t="n">
         <v>12272.48</v>
@@ -17714,25 +17714,25 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>1830.81</v>
+        <v>2431.43</v>
       </c>
       <c r="E42" t="n">
-        <v>1830.81</v>
+        <v>2431.43</v>
       </c>
       <c r="F42" t="n">
-        <v>1830.81</v>
+        <v>2431.43</v>
       </c>
       <c r="G42" t="n">
-        <v>1830.81</v>
+        <v>2431.43</v>
       </c>
       <c r="H42" t="n">
-        <v>23157.24</v>
+        <v>23502.49</v>
       </c>
       <c r="I42" t="n">
-        <v>23157.24</v>
+        <v>23502.49</v>
       </c>
       <c r="J42" t="n">
-        <v>23157.24</v>
+        <v>23502.49</v>
       </c>
       <c r="K42" t="n">
         <v>1</v>
@@ -17816,16 +17816,16 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="E44" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="F44" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="G44" t="n">
-        <v>79901.81</v>
+        <v>79747.96000000001</v>
       </c>
       <c r="H44" t="n">
         <v>166013.41</v>
@@ -17867,16 +17867,16 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="E45" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="F45" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="G45" t="n">
-        <v>9139.809999999999</v>
+        <v>9129.09</v>
       </c>
       <c r="H45" t="n">
         <v>86166.2</v>
@@ -17918,25 +17918,25 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="E46" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="F46" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="G46" t="n">
-        <v>1738.87</v>
+        <v>1749.36</v>
       </c>
       <c r="H46" t="n">
-        <v>21480.66</v>
+        <v>21416.84</v>
       </c>
       <c r="I46" t="n">
-        <v>21480.66</v>
+        <v>21416.84</v>
       </c>
       <c r="J46" t="n">
-        <v>21480.66</v>
+        <v>21416.84</v>
       </c>
       <c r="K46" t="n">
         <v>1</v>
@@ -18071,25 +18071,25 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="E49" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="F49" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="G49" t="n">
-        <v>269778042.61</v>
+        <v>270563366.83</v>
       </c>
       <c r="H49" t="n">
-        <v>55068304.14</v>
+        <v>55374839.99</v>
       </c>
       <c r="I49" t="n">
-        <v>55068304.14</v>
+        <v>55374839.99</v>
       </c>
       <c r="J49" t="n">
-        <v>55068304.14</v>
+        <v>55374839.99</v>
       </c>
       <c r="K49" t="n">
         <v>1</v>
@@ -18122,25 +18122,25 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="E50" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="F50" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="G50" t="n">
-        <v>5856.31</v>
+        <v>5980.47</v>
       </c>
       <c r="H50" t="n">
-        <v>59174.67</v>
+        <v>59068.31</v>
       </c>
       <c r="I50" t="n">
-        <v>59174.67</v>
+        <v>59068.31</v>
       </c>
       <c r="J50" t="n">
-        <v>59174.67</v>
+        <v>59068.31</v>
       </c>
       <c r="K50" t="n">
         <v>1</v>

</xml_diff>